<commit_message>
Added firmware flow diagram to spreadsheet.
Started rough firmware flow diagram for the code. Added it here to
be with the pin assignments etc.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Assignment" sheetId="1" r:id="rId1"/>
     <sheet name="STK600-RCUC3C0-36 Routing Card" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="FlowDiagram" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin Assignment'!$A$2:$J$153</definedName>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="527">
   <si>
     <t>PIN</t>
   </si>
@@ -1594,6 +1594,12 @@
   </si>
   <si>
     <t>SPI Data In from UC3C to Arduino</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2114,15 +2120,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2153,6 +2150,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2168,6 +2175,1744 @@
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Terminator 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="485775"/>
+          <a:ext cx="2266950" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>START</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Flowchart: Decision 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2266950" y="1943100"/>
+          <a:ext cx="3238500" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Configuration stored in</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> memory?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Flowchart: Process 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590801" y="4210050"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="6350"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Load configuration from</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>flash memory</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Flowchart: Process 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590801" y="6477000"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Execute QTouch Library Detection. On detect, set appropriate GPIO pin.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Flowchart: Decision 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2266950" y="8743950"/>
+          <a:ext cx="3238500" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Host MCU requests data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Elbow Connector 8"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3481388" y="1538287"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Elbow Connector 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3481388" y="3805236"/>
+          <a:ext cx="809625" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161133</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>796</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Elbow Connector 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3481389" y="6072187"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Elbow Connector 20"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3481389" y="8339137"/>
+          <a:ext cx="809625" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Elbow Connector 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="3"/>
+          <a:endCxn id="28" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5505450" y="9472613"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Flowchart: Decision 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315075" y="8743950"/>
+          <a:ext cx="3238500" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Host MCU want to reconfigure sensors</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Elbow Connector 29"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="0"/>
+          <a:endCxn id="6" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="5788820" y="6598445"/>
+          <a:ext cx="1538287" cy="2752724"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Elbow Connector 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="2"/>
+          <a:endCxn id="43" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3481388" y="10606087"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Elbow Connector 29"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="2"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="607220" y="9189245"/>
+          <a:ext cx="5262562" cy="1295399"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -4344"/>
+            <a:gd name="adj2" fmla="val 197794"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Flowchart: Predefined Process 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="11010900"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartPredefinedProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Reconfigure sensor</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>s</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Flowchart: Predefined Process 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590800" y="11010900"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartPredefinedProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Transfer requested</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> data</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Elbow Connector 48"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="2"/>
+          <a:endCxn id="42" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7529513" y="10606087"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Flowchart: Terminator 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6800850" y="17811750"/>
+          <a:ext cx="2266950" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>RESET MCU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Elbow Connector 52"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7529513" y="12873037"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Flowchart: Decision 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315075" y="13277850"/>
+          <a:ext cx="3238500" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Store</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> changes permanently to flash?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Flowchart: Predefined Process 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="15544800"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartPredefinedProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Store new configuration in </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>flash memory</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Elbow Connector 59"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="2"/>
+          <a:endCxn id="59" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7529513" y="15139987"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Elbow Connector 62"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="59" idx="2"/>
+          <a:endCxn id="52" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7529513" y="17406937"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Flowchart: Decision 65"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315075" y="1943100"/>
+          <a:ext cx="3238500" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Configuration being</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> sent by host MCU?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Flowchart: Predefined Process 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="4210050"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartPredefinedProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Store configuration</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> in SRAM; check validity of selected options. Save to flash if requested. Load configuration.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Elbow Connector 67"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="66" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5505450" y="2671763"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>161132</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>795</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Elbow Connector 70"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="66" idx="2"/>
+          <a:endCxn id="67" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7529513" y="3805237"/>
+          <a:ext cx="809625" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>3</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Elbow Connector 73"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="67" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5667377" y="3886201"/>
+          <a:ext cx="485775" cy="4048123"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Flowchart: Process 76"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10525125" y="1943100"/>
+          <a:ext cx="2590800" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="6350"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Wait</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Elbow Connector 77"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="66" idx="3"/>
+          <a:endCxn id="77" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9553575" y="2671763"/>
+          <a:ext cx="971550" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>794</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>794</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>794</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Elbow Connector 80"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="77" idx="0"/>
+          <a:endCxn id="66" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="9877425" y="0"/>
+          <a:ext cx="1588" cy="3886200"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 45585657"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2460,8 +4205,8 @@
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2477,51 +4222,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickTop="1" thickBot="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="44" t="s">
         <v>362</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" s="46" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="43" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="45"/>
+    </row>
+    <row r="2" spans="1:10" s="43" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>522</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="41" t="s">
         <v>359</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="42" t="s">
         <v>343</v>
       </c>
     </row>
@@ -6152,1072 +7897,1072 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" thickBot="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>388</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="35" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="37" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="37" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="37" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="37" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="37" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="37" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="37" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="37" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="37" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="37" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="37" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="37" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="37" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="37" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="37" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="37" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="36" t="s">
         <v>407</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="37" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="37" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="37" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="37" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="37" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="37" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="37" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="37" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="37" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="37" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="37" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="37" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="37" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="37" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="37" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="37" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="37" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="37" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="37" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="37" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="37" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="37" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="37" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="37" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="37" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="37" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="37" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B46" s="37" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="37" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="37" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="37" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="37" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="37" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="37" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="37" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="37" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="37" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="37" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="37" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="37" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="37" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="37" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="37" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="37" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="37" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A64" s="39" t="s">
+      <c r="A64" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="37" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="37" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A66" s="39" t="s">
+      <c r="A66" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="37" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="37" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="37" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A69" s="39" t="s">
+      <c r="A69" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="37" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="37" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="37" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="40" t="s">
+      <c r="B72" s="37" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="37" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="37" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="40" t="s">
+      <c r="B75" s="37" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A76" s="39" t="s">
+      <c r="A76" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B76" s="40" t="s">
+      <c r="B76" s="37" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A77" s="39" t="s">
+      <c r="A77" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B77" s="40" t="s">
+      <c r="B77" s="37" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="37" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="37" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="B80" s="40" t="s">
+      <c r="B80" s="37" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A81" s="39" t="s">
+      <c r="A81" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="37" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A82" s="39" t="s">
+      <c r="A82" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="37" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A83" s="39" t="s">
+      <c r="A83" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="40" t="s">
+      <c r="B83" s="37" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="37" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="B85" s="40" t="s">
+      <c r="B85" s="37" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A86" s="39" t="s">
+      <c r="A86" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="B86" s="40" t="s">
+      <c r="B86" s="37" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="B87" s="40" t="s">
+      <c r="B87" s="37" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A88" s="39" t="s">
+      <c r="A88" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="37" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A89" s="39" t="s">
+      <c r="A89" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="37" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="B90" s="40" t="s">
+      <c r="B90" s="37" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="B91" s="40" t="s">
+      <c r="B91" s="37" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A92" s="39" t="s">
+      <c r="A92" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="B92" s="40" t="s">
+      <c r="B92" s="37" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A93" s="39" t="s">
+      <c r="A93" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="37" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="B94" s="40" t="s">
+      <c r="B94" s="37" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A95" s="39" t="s">
+      <c r="A95" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="B95" s="40" t="s">
+      <c r="B95" s="37" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B96" s="40" t="s">
+      <c r="B96" s="37" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A97" s="39" t="s">
+      <c r="A97" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="B97" s="40" t="s">
+      <c r="B97" s="37" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A98" s="39" t="s">
+      <c r="A98" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B98" s="40" t="s">
+      <c r="B98" s="37" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B99" s="40" t="s">
+      <c r="B99" s="37" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="B100" s="40" t="s">
+      <c r="B100" s="37" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A101" s="39" t="s">
+      <c r="A101" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="37" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A102" s="39" t="s">
+      <c r="A102" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="37" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A103" s="39" t="s">
+      <c r="A103" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="B103" s="40" t="s">
+      <c r="B103" s="37" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A104" s="39" t="s">
+      <c r="A104" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="37" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A105" s="39" t="s">
+      <c r="A105" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="37" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A106" s="39" t="s">
+      <c r="A106" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="B106" s="40" t="s">
+      <c r="B106" s="37" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A107" s="39" t="s">
+      <c r="A107" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B107" s="40" t="s">
+      <c r="B107" s="37" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A108" s="39" t="s">
+      <c r="A108" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="37" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A109" s="39" t="s">
+      <c r="A109" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B109" s="40" t="s">
+      <c r="B109" s="37" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A110" s="39" t="s">
+      <c r="A110" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="37" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="B111" s="40" t="s">
+      <c r="B111" s="37" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A112" s="39" t="s">
+      <c r="A112" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B112" s="40" t="s">
+      <c r="B112" s="37" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="37" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B114" s="40" t="s">
+      <c r="B114" s="37" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A115" s="39" t="s">
+      <c r="A115" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="37" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A116" s="39" t="s">
+      <c r="A116" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="B116" s="40" t="s">
+      <c r="B116" s="37" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A117" s="39" t="s">
+      <c r="A117" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B117" s="40" t="s">
+      <c r="B117" s="37" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A118" s="39" t="s">
+      <c r="A118" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B118" s="40" t="s">
+      <c r="B118" s="37" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A119" s="39" t="s">
+      <c r="A119" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B119" s="40" t="s">
+      <c r="B119" s="37" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A120" s="39" t="s">
+      <c r="A120" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="B120" s="40" t="s">
+      <c r="B120" s="37" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A121" s="39" t="s">
+      <c r="A121" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B121" s="40" t="s">
+      <c r="B121" s="37" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A122" s="39" t="s">
+      <c r="A122" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B122" s="40" t="s">
+      <c r="B122" s="37" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B123" s="40" t="s">
+      <c r="B123" s="37" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A124" s="39" t="s">
+      <c r="A124" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="B124" s="40" t="s">
+      <c r="B124" s="37" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A125" s="39" t="s">
+      <c r="A125" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="B125" s="40" t="s">
+      <c r="B125" s="37" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A126" s="39" t="s">
+      <c r="A126" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="B126" s="40" t="s">
+      <c r="B126" s="37" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A127" s="39" t="s">
+      <c r="A127" s="36" t="s">
         <v>383</v>
       </c>
-      <c r="B127" s="40" t="s">
+      <c r="B127" s="37" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A128" s="39" t="s">
+      <c r="A128" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B128" s="40" t="s">
+      <c r="B128" s="37" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A129" s="39" t="s">
+      <c r="A129" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B129" s="40" t="s">
+      <c r="B129" s="37" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A130" s="39" t="s">
+      <c r="A130" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B130" s="40" t="s">
+      <c r="B130" s="37" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A131" s="39" t="s">
+      <c r="A131" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B131" s="40" t="s">
+      <c r="B131" s="37" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A132" s="39" t="s">
+      <c r="A132" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B132" s="40"/>
+      <c r="B132" s="37"/>
     </row>
     <row r="133" spans="1:2" ht="17.25" thickBot="1">
-      <c r="A133" s="39" t="s">
+      <c r="A133" s="36" t="s">
         <v>521</v>
       </c>
-      <c r="B133" s="40" t="s">
+      <c r="B133" s="37" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="16.5">
-      <c r="A134" s="41" t="s">
+      <c r="A134" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B134" s="42" t="s">
+      <c r="B134" s="39" t="s">
         <v>225</v>
       </c>
     </row>
@@ -7229,12 +8974,60 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="Z16:BH92"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L22" workbookViewId="0">
+      <selection activeCell="BH45" sqref="BH45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetData>
+    <row r="16" spans="35:60" ht="12.75" customHeight="1">
+      <c r="AI16" s="47" t="s">
+        <v>526</v>
+      </c>
+      <c r="BH16" s="47" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="22" spans="26:51" ht="12.75" customHeight="1">
+      <c r="Z22" s="47" t="s">
+        <v>525</v>
+      </c>
+      <c r="AY22" s="47" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="54" spans="26:51" ht="12.75" customHeight="1">
+      <c r="AY54" s="47" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="58" spans="26:51" ht="12.75" customHeight="1">
+      <c r="AI58" s="47" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="64" spans="26:51" ht="12.75" customHeight="1">
+      <c r="Z64" s="47" t="s">
+        <v>525</v>
+      </c>
+      <c r="AY64" s="47" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="86" spans="51:60" ht="12.75" customHeight="1">
+      <c r="BH86" s="47" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="92" spans="51:60" ht="12.75" customHeight="1">
+      <c r="AY92" s="47" t="s">
+        <v>525</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified naming of detect pins as being "per sensor".
In keeping with the whole QTouch library, the detect pins are now
named as being "per sensor", since a slider or rotor takes up 3
channels which make up 1 sensor.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Assignment" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="528">
   <si>
     <t>PIN</t>
   </si>
@@ -843,198 +843,6 @@
     <t>Connect to X.XkOhn resistor -&gt; header with local header pin for GND of sensor wiring</t>
   </si>
   <si>
-    <t>DETECT_CH00</t>
-  </si>
-  <si>
-    <t>DETECT_CH01</t>
-  </si>
-  <si>
-    <t>DETECT_CH02</t>
-  </si>
-  <si>
-    <t>DETECT_CH03</t>
-  </si>
-  <si>
-    <t>DETECT_CH04</t>
-  </si>
-  <si>
-    <t>DETECT_CH05</t>
-  </si>
-  <si>
-    <t>DETECT_CH06</t>
-  </si>
-  <si>
-    <t>DETECT_CH07</t>
-  </si>
-  <si>
-    <t>DETECT_CH08</t>
-  </si>
-  <si>
-    <t>DETECT_CH09</t>
-  </si>
-  <si>
-    <t>DETECT_CH10</t>
-  </si>
-  <si>
-    <t>DETECT_CH11</t>
-  </si>
-  <si>
-    <t>DETECT_CH12</t>
-  </si>
-  <si>
-    <t>DETECT_CH13</t>
-  </si>
-  <si>
-    <t>DETECT_CH14</t>
-  </si>
-  <si>
-    <t>DETECT_CH15</t>
-  </si>
-  <si>
-    <t>DETECT_CH16</t>
-  </si>
-  <si>
-    <t>DETECT_CH17</t>
-  </si>
-  <si>
-    <t>DETECT_CH18</t>
-  </si>
-  <si>
-    <t>DETECT_CH19</t>
-  </si>
-  <si>
-    <t>DETECT_CH20</t>
-  </si>
-  <si>
-    <t>DETECT_CH21</t>
-  </si>
-  <si>
-    <t>DETECT_CH22</t>
-  </si>
-  <si>
-    <t>DETECT_CH23</t>
-  </si>
-  <si>
-    <t>DETECT_CH24</t>
-  </si>
-  <si>
-    <t>DETECT_CH25</t>
-  </si>
-  <si>
-    <t>DETECT_CH26</t>
-  </si>
-  <si>
-    <t>DETECT_CH27</t>
-  </si>
-  <si>
-    <t>DETECT_CH28</t>
-  </si>
-  <si>
-    <t>DETECT_CH29</t>
-  </si>
-  <si>
-    <t>DETECT_CH30</t>
-  </si>
-  <si>
-    <t>DETECT_CH31</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 00</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 01</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 02</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 03</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 04</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 05</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 06</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 07</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 08</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 09</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 10</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 12</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 13</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 14</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 15</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 16</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 17</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 18</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 19</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 20</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 21</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 11</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 22</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 23</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 24</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 25</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 26</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 27</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 28</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 29</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 30</t>
-  </si>
-  <si>
-    <t>Digital output for sense detect on channel 31</t>
-  </si>
-  <si>
     <t>Connect via X.XnF capacitor to SNSK00</t>
   </si>
   <si>
@@ -1095,9 +903,6 @@
     <t>QT-SENSE-KEY</t>
   </si>
   <si>
-    <t>SHIELD-DETECT</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -1600,6 +1405,204 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>SHIELD-DETECT-OUTPUT</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR00</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR01</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR02</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR03</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR04</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR05</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR06</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR07</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR08</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR09</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR10</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR11</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR12</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR13</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR14</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR15</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR16</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR17</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR18</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR19</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR20</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR21</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR22</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR23</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR24</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR25</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR26</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR27</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR28</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR29</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR30</t>
+  </si>
+  <si>
+    <t>DETECT-SENSOR31</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 00</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 01</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 02</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 03</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 04</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 05</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 06</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 07</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 08</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 09</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 10</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 11</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 12</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 13</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 14</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 15</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 16</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 17</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 18</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 19</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 20</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 21</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 22</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 23</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 24</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 25</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 26</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 27</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 28</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 29</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 30</t>
+  </si>
+  <si>
+    <t>Digital output for detection on sensor 31</t>
+  </si>
+  <si>
+    <t>??? Perhaps use for USB firmware upgrade ???</t>
   </si>
 </sst>
 </file>
@@ -4205,16 +4208,16 @@
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="25.5703125" style="1" customWidth="1"/>
@@ -4223,12 +4226,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickTop="1" thickBot="1">
       <c r="A1" s="44" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="11"/>
       <c r="D1" s="44" t="s">
-        <v>362</v>
+        <v>297</v>
       </c>
       <c r="E1" s="46"/>
       <c r="F1" s="45"/>
@@ -4246,16 +4249,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>522</v>
+        <v>457</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>351</v>
+        <v>287</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>359</v>
+        <v>294</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>7</v>
@@ -4267,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="42" t="s">
-        <v>343</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1">
@@ -4285,7 +4288,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="14"/>
@@ -4307,7 +4310,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
@@ -4329,7 +4332,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -4351,7 +4354,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="18"/>
@@ -4370,13 +4373,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>224</v>
@@ -4398,13 +4401,13 @@
         <v>17</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>225</v>
@@ -4426,7 +4429,7 @@
         <v>166</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>220</v>
@@ -4450,7 +4453,7 @@
         <v>167</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>220</v>
@@ -4474,7 +4477,7 @@
         <v>168</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>220</v>
@@ -4498,7 +4501,7 @@
         <v>169</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>220</v>
@@ -4522,7 +4525,7 @@
         <v>170</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>220</v>
@@ -4546,7 +4549,7 @@
         <v>171</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>220</v>
@@ -4570,7 +4573,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>220</v>
@@ -4594,7 +4597,7 @@
         <v>46</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>220</v>
@@ -4618,7 +4621,7 @@
         <v>47</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>220</v>
@@ -4642,7 +4645,7 @@
         <v>48</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>220</v>
@@ -4666,7 +4669,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>220</v>
@@ -4690,7 +4693,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>220</v>
@@ -4714,7 +4717,7 @@
         <v>51</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>220</v>
@@ -4738,7 +4741,7 @@
         <v>52</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>220</v>
@@ -4762,10 +4765,10 @@
         <v>241</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>354</v>
+        <v>290</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>363</v>
+        <v>298</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
@@ -4786,10 +4789,10 @@
         <v>242</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>364</v>
+        <v>299</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
@@ -4807,13 +4810,13 @@
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
-        <v>274</v>
+        <v>463</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>306</v>
+        <v>495</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
@@ -4829,13 +4832,13 @@
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18" t="s">
-        <v>275</v>
+        <v>464</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>307</v>
+        <v>496</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
@@ -4851,13 +4854,13 @@
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18" t="s">
-        <v>276</v>
+        <v>465</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>308</v>
+        <v>497</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
@@ -4873,13 +4876,13 @@
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
-        <v>277</v>
+        <v>466</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>309</v>
+        <v>498</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
@@ -4895,13 +4898,13 @@
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
-        <v>278</v>
+        <v>467</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>310</v>
+        <v>499</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
@@ -4917,13 +4920,13 @@
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18" t="s">
-        <v>279</v>
+        <v>468</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>311</v>
+        <v>500</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
@@ -4939,13 +4942,13 @@
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="s">
-        <v>280</v>
+        <v>469</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>312</v>
+        <v>501</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -4961,13 +4964,13 @@
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18" t="s">
-        <v>281</v>
+        <v>470</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>313</v>
+        <v>502</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
@@ -4983,13 +4986,13 @@
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18" t="s">
-        <v>282</v>
+        <v>471</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>314</v>
+        <v>503</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -5005,13 +5008,13 @@
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
-        <v>283</v>
+        <v>472</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>315</v>
+        <v>504</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
@@ -5027,13 +5030,13 @@
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18" t="s">
-        <v>284</v>
+        <v>473</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>316</v>
+        <v>505</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -5052,14 +5055,14 @@
         <v>238</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
       <c r="J36" s="20" t="s">
-        <v>365</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -5074,14 +5077,14 @@
         <v>238</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
       <c r="J37" s="20" t="s">
-        <v>366</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -5093,13 +5096,13 @@
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18" t="s">
-        <v>285</v>
+        <v>474</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>327</v>
+        <v>506</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
@@ -5118,13 +5121,13 @@
         <v>17</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H39" s="23" t="s">
         <v>225</v>
@@ -5133,7 +5136,7 @@
         <v>225</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>346</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -5148,13 +5151,13 @@
         <v>15</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H40" s="23" t="s">
         <v>224</v>
@@ -5163,7 +5166,7 @@
         <v>224</v>
       </c>
       <c r="J40" s="24" t="s">
-        <v>345</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -5175,13 +5178,13 @@
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="23" t="s">
-        <v>286</v>
+        <v>475</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>317</v>
+        <v>507</v>
       </c>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
@@ -5197,13 +5200,13 @@
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="23" t="s">
-        <v>287</v>
+        <v>476</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>318</v>
+        <v>508</v>
       </c>
       <c r="G42" s="23"/>
       <c r="H42" s="23"/>
@@ -5219,13 +5222,13 @@
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
-        <v>288</v>
+        <v>477</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>319</v>
+        <v>509</v>
       </c>
       <c r="G43" s="23"/>
       <c r="H43" s="23"/>
@@ -5241,13 +5244,13 @@
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="23" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>320</v>
+        <v>510</v>
       </c>
       <c r="G44" s="23"/>
       <c r="H44" s="23"/>
@@ -5263,13 +5266,13 @@
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="23" t="s">
-        <v>290</v>
+        <v>479</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>321</v>
+        <v>511</v>
       </c>
       <c r="G45" s="23"/>
       <c r="H45" s="23"/>
@@ -5285,13 +5288,13 @@
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="23" t="s">
-        <v>291</v>
+        <v>480</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>322</v>
+        <v>512</v>
       </c>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -5307,13 +5310,13 @@
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="23" t="s">
-        <v>292</v>
+        <v>481</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>323</v>
+        <v>513</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="23"/>
@@ -5329,13 +5332,13 @@
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="23" t="s">
-        <v>293</v>
+        <v>482</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>324</v>
+        <v>514</v>
       </c>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -5351,13 +5354,13 @@
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="23" t="s">
-        <v>294</v>
+        <v>483</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>325</v>
+        <v>515</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="23"/>
@@ -5373,13 +5376,13 @@
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="23" t="s">
-        <v>295</v>
+        <v>484</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>326</v>
+        <v>516</v>
       </c>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -5398,11 +5401,11 @@
         <v>17</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H51" s="23" t="s">
         <v>225</v>
@@ -5411,7 +5414,7 @@
         <v>225</v>
       </c>
       <c r="J51" s="24" t="s">
-        <v>386</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -5426,13 +5429,15 @@
         <v>238</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F52" s="23"/>
       <c r="G52" s="23"/>
       <c r="H52" s="23"/>
       <c r="I52" s="25"/>
-      <c r="J52" s="24"/>
+      <c r="J52" s="24" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="22">
@@ -5446,13 +5451,15 @@
         <v>238</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F53" s="23"/>
       <c r="G53" s="23"/>
       <c r="H53" s="23"/>
       <c r="I53" s="25"/>
-      <c r="J53" s="24"/>
+      <c r="J53" s="24" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="22">
@@ -5466,11 +5473,11 @@
         <v>17</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H54" s="23" t="s">
         <v>225</v>
@@ -5492,11 +5499,11 @@
         <v>15</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H55" s="23" t="s">
         <v>224</v>
@@ -5515,16 +5522,16 @@
       </c>
       <c r="C56" s="23"/>
       <c r="D56" s="23" t="s">
-        <v>347</v>
+        <v>283</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>368</v>
+        <v>303</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H56" s="23" t="s">
         <v>225</v>
@@ -5533,7 +5540,7 @@
         <v>225</v>
       </c>
       <c r="J56" s="24" t="s">
-        <v>344</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -5545,16 +5552,16 @@
       </c>
       <c r="C57" s="23"/>
       <c r="D57" s="23" t="s">
-        <v>347</v>
+        <v>283</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>368</v>
+        <v>303</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H57" s="23" t="s">
         <v>225</v>
@@ -5563,7 +5570,7 @@
         <v>225</v>
       </c>
       <c r="J57" s="24" t="s">
-        <v>344</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -5578,11 +5585,11 @@
         <v>17</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="23" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H58" s="23" t="s">
         <v>225</v>
@@ -5604,7 +5611,7 @@
         <v>173</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F59" s="23" t="s">
         <v>220</v>
@@ -5628,7 +5635,7 @@
         <v>174</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F60" s="23" t="s">
         <v>220</v>
@@ -5652,7 +5659,7 @@
         <v>175</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F61" s="23" t="s">
         <v>220</v>
@@ -5676,7 +5683,7 @@
         <v>176</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F62" s="23" t="s">
         <v>220</v>
@@ -5700,7 +5707,7 @@
         <v>177</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F63" s="23" t="s">
         <v>220</v>
@@ -5724,7 +5731,7 @@
         <v>178</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F64" s="23" t="s">
         <v>220</v>
@@ -5748,7 +5755,7 @@
         <v>179</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F65" s="23" t="s">
         <v>220</v>
@@ -5772,7 +5779,7 @@
         <v>180</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F66" s="23" t="s">
         <v>220</v>
@@ -5796,7 +5803,7 @@
         <v>181</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F67" s="23" t="s">
         <v>220</v>
@@ -5820,7 +5827,7 @@
         <v>182</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F68" s="23" t="s">
         <v>220</v>
@@ -5844,7 +5851,7 @@
         <v>183</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F69" s="23" t="s">
         <v>220</v>
@@ -5868,7 +5875,7 @@
         <v>184</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F70" s="23" t="s">
         <v>220</v>
@@ -5892,7 +5899,7 @@
         <v>185</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F71" s="23" t="s">
         <v>220</v>
@@ -5916,7 +5923,7 @@
         <v>186</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F72" s="23" t="s">
         <v>220</v>
@@ -5940,7 +5947,7 @@
         <v>187</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F73" s="23" t="s">
         <v>219</v>
@@ -5964,7 +5971,7 @@
         <v>188</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F74" s="23" t="s">
         <v>219</v>
@@ -5988,7 +5995,7 @@
         <v>189</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F75" s="27" t="s">
         <v>219</v>
@@ -6012,7 +6019,7 @@
         <v>190</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>219</v>
@@ -6036,13 +6043,13 @@
         <v>15</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G77" s="27" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H77" s="27" t="s">
         <v>224</v>
@@ -6064,13 +6071,13 @@
         <v>17</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F78" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H78" s="27" t="s">
         <v>225</v>
@@ -6092,7 +6099,7 @@
         <v>191</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F79" s="27" t="s">
         <v>219</v>
@@ -6116,7 +6123,7 @@
         <v>192</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F80" s="27" t="s">
         <v>219</v>
@@ -6140,7 +6147,7 @@
         <v>193</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F81" s="27" t="s">
         <v>219</v>
@@ -6164,7 +6171,7 @@
         <v>194</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F82" s="27" t="s">
         <v>219</v>
@@ -6188,7 +6195,7 @@
         <v>195</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F83" s="27" t="s">
         <v>219</v>
@@ -6212,7 +6219,7 @@
         <v>196</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F84" s="27" t="s">
         <v>219</v>
@@ -6236,7 +6243,7 @@
         <v>197</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F85" s="27" t="s">
         <v>219</v>
@@ -6260,7 +6267,7 @@
         <v>198</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F86" s="27" t="s">
         <v>219</v>
@@ -6284,7 +6291,7 @@
         <v>199</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F87" s="27" t="s">
         <v>219</v>
@@ -6308,7 +6315,7 @@
         <v>200</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F88" s="27" t="s">
         <v>219</v>
@@ -6332,7 +6339,7 @@
         <v>201</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F89" s="27" t="s">
         <v>219</v>
@@ -6356,7 +6363,7 @@
         <v>202</v>
       </c>
       <c r="E90" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F90" s="27" t="s">
         <v>219</v>
@@ -6380,7 +6387,7 @@
         <v>203</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F91" s="27" t="s">
         <v>219</v>
@@ -6404,7 +6411,7 @@
         <v>204</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F92" s="27" t="s">
         <v>219</v>
@@ -6428,7 +6435,7 @@
         <v>205</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F93" s="27" t="s">
         <v>219</v>
@@ -6452,7 +6459,7 @@
         <v>206</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F94" s="27" t="s">
         <v>219</v>
@@ -6476,7 +6483,7 @@
         <v>207</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F95" s="27" t="s">
         <v>219</v>
@@ -6500,7 +6507,7 @@
         <v>208</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F96" s="27" t="s">
         <v>219</v>
@@ -6524,7 +6531,7 @@
         <v>209</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F97" s="27" t="s">
         <v>219</v>
@@ -6548,7 +6555,7 @@
         <v>210</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F98" s="27" t="s">
         <v>219</v>
@@ -6572,7 +6579,7 @@
         <v>211</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F99" s="27" t="s">
         <v>219</v>
@@ -6596,7 +6603,7 @@
         <v>212</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F100" s="27" t="s">
         <v>219</v>
@@ -6620,7 +6627,7 @@
         <v>213</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F101" s="27" t="s">
         <v>219</v>
@@ -6644,7 +6651,7 @@
         <v>214</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F102" s="27" t="s">
         <v>219</v>
@@ -6668,7 +6675,7 @@
         <v>215</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F103" s="27" t="s">
         <v>219</v>
@@ -6692,7 +6699,7 @@
         <v>216</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F104" s="27" t="s">
         <v>219</v>
@@ -6716,13 +6723,13 @@
         <v>15</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F105" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G105" s="27" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H105" s="27" t="s">
         <v>224</v>
@@ -6744,13 +6751,13 @@
         <v>17</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F106" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G106" s="27" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H106" s="27" t="s">
         <v>225</v>
@@ -6772,7 +6779,7 @@
         <v>217</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F107" s="27" t="s">
         <v>219</v>
@@ -6796,7 +6803,7 @@
         <v>218</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="F108" s="27" t="s">
         <v>219</v>
@@ -6820,16 +6827,16 @@
         <v>221</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F109" s="27" t="s">
         <v>236</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H109" s="27" t="s">
-        <v>370</v>
+        <v>305</v>
       </c>
       <c r="I109" s="28">
         <v>18</v>
@@ -6848,16 +6855,16 @@
         <v>222</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F110" s="27" t="s">
         <v>235</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H110" s="27" t="s">
-        <v>371</v>
+        <v>306</v>
       </c>
       <c r="I110" s="28">
         <v>19</v>
@@ -6873,19 +6880,19 @@
       </c>
       <c r="C111" s="31"/>
       <c r="D111" s="31" t="s">
-        <v>348</v>
+        <v>284</v>
       </c>
       <c r="E111" s="31" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>349</v>
+        <v>285</v>
       </c>
       <c r="G111" s="31"/>
       <c r="H111" s="31"/>
       <c r="I111" s="32"/>
       <c r="J111" s="33" t="s">
-        <v>372</v>
+        <v>307</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -6896,19 +6903,19 @@
         <v>129</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>489</v>
+        <v>424</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>226</v>
       </c>
       <c r="E112" s="31" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F112" s="31" t="s">
         <v>234</v>
       </c>
       <c r="G112" s="31" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="H112" s="31" t="s">
         <v>227</v>
@@ -6928,19 +6935,19 @@
         <v>130</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>490</v>
+        <v>425</v>
       </c>
       <c r="D113" s="31" t="s">
         <v>228</v>
       </c>
       <c r="E113" s="31" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F113" s="31" t="s">
-        <v>523</v>
+        <v>458</v>
       </c>
       <c r="G113" s="31" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="H113" s="31" t="s">
         <v>231</v>
@@ -6960,19 +6967,19 @@
         <v>131</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>491</v>
+        <v>426</v>
       </c>
       <c r="D114" s="31" t="s">
         <v>230</v>
       </c>
       <c r="E114" s="31" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F114" s="31" t="s">
-        <v>524</v>
+        <v>459</v>
       </c>
       <c r="G114" s="31" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="H114" s="31" t="s">
         <v>229</v>
@@ -6992,19 +6999,19 @@
         <v>132</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>492</v>
+        <v>427</v>
       </c>
       <c r="D115" s="31" t="s">
         <v>232</v>
       </c>
       <c r="E115" s="31" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F115" s="31" t="s">
         <v>233</v>
       </c>
       <c r="G115" s="31" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="H115" s="31" t="s">
         <v>237</v>
@@ -7028,7 +7035,7 @@
         <v>238</v>
       </c>
       <c r="E116" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F116" s="31"/>
       <c r="G116" s="31"/>
@@ -7048,7 +7055,7 @@
         <v>238</v>
       </c>
       <c r="E117" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F117" s="31"/>
       <c r="G117" s="31"/>
@@ -7068,7 +7075,7 @@
         <v>238</v>
       </c>
       <c r="E118" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F118" s="31"/>
       <c r="G118" s="31"/>
@@ -7088,7 +7095,7 @@
         <v>238</v>
       </c>
       <c r="E119" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F119" s="31"/>
       <c r="G119" s="31"/>
@@ -7108,13 +7115,13 @@
         <v>15</v>
       </c>
       <c r="E120" s="31" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F120" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G120" s="31" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H120" s="31" t="s">
         <v>224</v>
@@ -7136,13 +7143,13 @@
         <v>17</v>
       </c>
       <c r="E121" s="31" t="s">
-        <v>352</v>
+        <v>288</v>
       </c>
       <c r="F121" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G121" s="31" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H121" s="31" t="s">
         <v>225</v>
@@ -7161,13 +7168,13 @@
       </c>
       <c r="C122" s="31"/>
       <c r="D122" s="31" t="s">
-        <v>296</v>
+        <v>485</v>
       </c>
       <c r="E122" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>328</v>
+        <v>517</v>
       </c>
       <c r="G122" s="31"/>
       <c r="H122" s="31"/>
@@ -7183,13 +7190,13 @@
       </c>
       <c r="C123" s="31"/>
       <c r="D123" s="31" t="s">
-        <v>297</v>
+        <v>486</v>
       </c>
       <c r="E123" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>329</v>
+        <v>518</v>
       </c>
       <c r="G123" s="31"/>
       <c r="H123" s="31"/>
@@ -7205,13 +7212,13 @@
       </c>
       <c r="C124" s="31"/>
       <c r="D124" s="31" t="s">
-        <v>298</v>
+        <v>487</v>
       </c>
       <c r="E124" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>330</v>
+        <v>519</v>
       </c>
       <c r="G124" s="31"/>
       <c r="H124" s="31"/>
@@ -7227,13 +7234,13 @@
       </c>
       <c r="C125" s="31"/>
       <c r="D125" s="31" t="s">
-        <v>299</v>
+        <v>488</v>
       </c>
       <c r="E125" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>331</v>
+        <v>520</v>
       </c>
       <c r="G125" s="31"/>
       <c r="H125" s="31"/>
@@ -7249,13 +7256,13 @@
       </c>
       <c r="C126" s="31"/>
       <c r="D126" s="31" t="s">
-        <v>300</v>
+        <v>489</v>
       </c>
       <c r="E126" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F126" s="31" t="s">
-        <v>332</v>
+        <v>521</v>
       </c>
       <c r="G126" s="31"/>
       <c r="H126" s="31"/>
@@ -7271,13 +7278,13 @@
       </c>
       <c r="C127" s="31"/>
       <c r="D127" s="31" t="s">
-        <v>301</v>
+        <v>490</v>
       </c>
       <c r="E127" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F127" s="31" t="s">
-        <v>333</v>
+        <v>522</v>
       </c>
       <c r="G127" s="31"/>
       <c r="H127" s="31"/>
@@ -7293,13 +7300,13 @@
       </c>
       <c r="C128" s="31"/>
       <c r="D128" s="31" t="s">
-        <v>302</v>
+        <v>491</v>
       </c>
       <c r="E128" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F128" s="31" t="s">
-        <v>334</v>
+        <v>523</v>
       </c>
       <c r="G128" s="31"/>
       <c r="H128" s="31"/>
@@ -7315,13 +7322,13 @@
       </c>
       <c r="C129" s="31"/>
       <c r="D129" s="31" t="s">
-        <v>303</v>
+        <v>492</v>
       </c>
       <c r="E129" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>335</v>
+        <v>524</v>
       </c>
       <c r="G129" s="31"/>
       <c r="H129" s="31"/>
@@ -7337,13 +7344,13 @@
       </c>
       <c r="C130" s="31"/>
       <c r="D130" s="31" t="s">
-        <v>304</v>
+        <v>493</v>
       </c>
       <c r="E130" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>336</v>
+        <v>525</v>
       </c>
       <c r="G130" s="31"/>
       <c r="H130" s="31"/>
@@ -7359,13 +7366,13 @@
       </c>
       <c r="C131" s="31"/>
       <c r="D131" s="31" t="s">
-        <v>305</v>
+        <v>494</v>
       </c>
       <c r="E131" s="31" t="s">
-        <v>358</v>
+        <v>462</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>337</v>
+        <v>526</v>
       </c>
       <c r="G131" s="31"/>
       <c r="H131" s="31"/>
@@ -7384,7 +7391,7 @@
         <v>238</v>
       </c>
       <c r="E132" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F132" s="31"/>
       <c r="G132" s="31"/>
@@ -7404,7 +7411,7 @@
         <v>238</v>
       </c>
       <c r="E133" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F133" s="31"/>
       <c r="G133" s="31"/>
@@ -7424,7 +7431,7 @@
         <v>238</v>
       </c>
       <c r="E134" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F134" s="31"/>
       <c r="G134" s="31"/>
@@ -7444,7 +7451,7 @@
         <v>238</v>
       </c>
       <c r="E135" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F135" s="31"/>
       <c r="G135" s="31"/>
@@ -7464,7 +7471,7 @@
         <v>238</v>
       </c>
       <c r="E136" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F136" s="31"/>
       <c r="G136" s="31"/>
@@ -7484,7 +7491,7 @@
         <v>238</v>
       </c>
       <c r="E137" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F137" s="31"/>
       <c r="G137" s="31"/>
@@ -7504,7 +7511,7 @@
         <v>238</v>
       </c>
       <c r="E138" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F138" s="31"/>
       <c r="G138" s="31"/>
@@ -7524,7 +7531,7 @@
         <v>238</v>
       </c>
       <c r="E139" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F139" s="31"/>
       <c r="G139" s="31"/>
@@ -7544,7 +7551,7 @@
         <v>238</v>
       </c>
       <c r="E140" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F140" s="31"/>
       <c r="G140" s="31"/>
@@ -7564,7 +7571,7 @@
         <v>238</v>
       </c>
       <c r="E141" s="31" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="F141" s="31"/>
       <c r="G141" s="31"/>
@@ -7584,7 +7591,7 @@
         <v>163</v>
       </c>
       <c r="E142" s="31" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F142" s="31" t="s">
         <v>220</v>
@@ -7593,7 +7600,7 @@
       <c r="H142" s="31"/>
       <c r="I142" s="32"/>
       <c r="J142" s="33" t="s">
-        <v>338</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -7608,7 +7615,7 @@
         <v>162</v>
       </c>
       <c r="E143" s="31" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F143" s="31" t="s">
         <v>220</v>
@@ -7617,7 +7624,7 @@
       <c r="H143" s="31"/>
       <c r="I143" s="32"/>
       <c r="J143" s="33" t="s">
-        <v>339</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -7635,13 +7642,13 @@
         <v>8</v>
       </c>
       <c r="F144" s="31" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="G144" s="31"/>
       <c r="H144" s="31"/>
       <c r="I144" s="32"/>
       <c r="J144" s="33" t="s">
-        <v>342</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -7656,7 +7663,7 @@
         <v>164</v>
       </c>
       <c r="E145" s="31" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F145" s="31" t="s">
         <v>220</v>
@@ -7665,7 +7672,7 @@
       <c r="H145" s="31"/>
       <c r="I145" s="32"/>
       <c r="J145" s="33" t="s">
-        <v>340</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -7680,7 +7687,7 @@
         <v>165</v>
       </c>
       <c r="E146" s="31" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="F146" s="31" t="s">
         <v>220</v>
@@ -7689,7 +7696,7 @@
       <c r="H146" s="31"/>
       <c r="I146" s="32"/>
       <c r="J146" s="33" t="s">
-        <v>341</v>
+        <v>277</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -7698,22 +7705,22 @@
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>381</v>
+        <v>316</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>373</v>
+        <v>308</v>
       </c>
       <c r="I147" s="5">
         <v>17</v>
       </c>
       <c r="J147" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -7722,22 +7729,22 @@
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>382</v>
+        <v>317</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>374</v>
+        <v>309</v>
       </c>
       <c r="I148" s="5">
         <v>16</v>
       </c>
       <c r="J148" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -7746,22 +7753,22 @@
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>381</v>
+        <v>316</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>375</v>
+        <v>310</v>
       </c>
       <c r="I149" s="5">
         <v>15</v>
       </c>
       <c r="J149" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -7770,22 +7777,22 @@
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>382</v>
+        <v>317</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>376</v>
+        <v>311</v>
       </c>
       <c r="I150" s="5">
         <v>14</v>
       </c>
       <c r="J150" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -7794,22 +7801,22 @@
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>381</v>
+        <v>316</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>377</v>
+        <v>312</v>
       </c>
       <c r="I151" s="5">
         <v>0</v>
       </c>
       <c r="J151" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -7818,22 +7825,22 @@
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>382</v>
+        <v>317</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>378</v>
+        <v>313</v>
       </c>
       <c r="I152" s="5">
         <v>1</v>
       </c>
       <c r="J152" s="4" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:10" ht="15.75" thickBot="1">
@@ -7842,26 +7849,26 @@
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7" t="s">
-        <v>383</v>
+        <v>318</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>384</v>
+        <v>319</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>383</v>
+        <v>318</v>
       </c>
       <c r="I153" s="8"/>
       <c r="J153" s="9" t="s">
-        <v>385</v>
+        <v>320</v>
       </c>
     </row>
     <row r="154" spans="1:10" ht="15.75" thickTop="1"/>
     <row r="155" spans="1:10">
       <c r="A155" s="10" t="s">
-        <v>387</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -7898,10 +7905,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" thickBot="1">
       <c r="A1" s="34" t="s">
-        <v>388</v>
+        <v>323</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>389</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" thickBot="1">
@@ -7909,7 +7916,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>390</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" thickBot="1">
@@ -7917,7 +7924,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>391</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" thickBot="1">
@@ -7925,7 +7932,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>392</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" thickBot="1">
@@ -7933,7 +7940,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>393</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" thickBot="1">
@@ -7941,7 +7948,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>394</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" thickBot="1">
@@ -7949,7 +7956,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>395</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" thickBot="1">
@@ -7957,7 +7964,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>396</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" thickBot="1">
@@ -7965,7 +7972,7 @@
         <v>35</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>397</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" thickBot="1">
@@ -7973,7 +7980,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>398</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" thickBot="1">
@@ -7981,7 +7988,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>399</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" thickBot="1">
@@ -7989,7 +7996,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>400</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" thickBot="1">
@@ -7997,7 +8004,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>401</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" thickBot="1">
@@ -8005,7 +8012,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>402</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" thickBot="1">
@@ -8013,7 +8020,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>403</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" thickBot="1">
@@ -8021,7 +8028,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>404</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" thickBot="1">
@@ -8029,7 +8036,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>405</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" thickBot="1">
@@ -8037,23 +8044,23 @@
         <v>44</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>406</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" thickBot="1">
       <c r="A19" s="36" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>408</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" thickBot="1">
       <c r="A20" s="36" t="s">
-        <v>409</v>
+        <v>344</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>410</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" thickBot="1">
@@ -8061,7 +8068,7 @@
         <v>55</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>411</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" thickBot="1">
@@ -8069,7 +8076,7 @@
         <v>58</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>412</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" thickBot="1">
@@ -8077,7 +8084,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>413</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" thickBot="1">
@@ -8085,7 +8092,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>414</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" thickBot="1">
@@ -8093,7 +8100,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>415</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" thickBot="1">
@@ -8101,7 +8108,7 @@
         <v>62</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>416</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" thickBot="1">
@@ -8109,7 +8116,7 @@
         <v>63</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>417</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" thickBot="1">
@@ -8117,7 +8124,7 @@
         <v>64</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>418</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" thickBot="1">
@@ -8125,7 +8132,7 @@
         <v>65</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>419</v>
+        <v>354</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" thickBot="1">
@@ -8133,7 +8140,7 @@
         <v>66</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>420</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" thickBot="1">
@@ -8141,7 +8148,7 @@
         <v>67</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>421</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" thickBot="1">
@@ -8149,7 +8156,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>422</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" thickBot="1">
@@ -8157,7 +8164,7 @@
         <v>158</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>423</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" thickBot="1">
@@ -8165,7 +8172,7 @@
         <v>160</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>424</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" thickBot="1">
@@ -8173,7 +8180,7 @@
         <v>161</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>425</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" thickBot="1">
@@ -8181,7 +8188,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>426</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" thickBot="1">
@@ -8189,7 +8196,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>427</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.25" thickBot="1">
@@ -8197,7 +8204,7 @@
         <v>20</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>428</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.25" thickBot="1">
@@ -8205,7 +8212,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>429</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17.25" thickBot="1">
@@ -8213,7 +8220,7 @@
         <v>22</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>430</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.25" thickBot="1">
@@ -8221,7 +8228,7 @@
         <v>23</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>431</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" thickBot="1">
@@ -8229,7 +8236,7 @@
         <v>24</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>432</v>
+        <v>367</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.25" thickBot="1">
@@ -8237,7 +8244,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>433</v>
+        <v>368</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17.25" thickBot="1">
@@ -8245,7 +8252,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>434</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17.25" thickBot="1">
@@ -8253,7 +8260,7 @@
         <v>27</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>435</v>
+        <v>370</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" thickBot="1">
@@ -8261,7 +8268,7 @@
         <v>28</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>436</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" thickBot="1">
@@ -8269,7 +8276,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>437</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.25" thickBot="1">
@@ -8277,7 +8284,7 @@
         <v>30</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>438</v>
+        <v>373</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.25" thickBot="1">
@@ -8285,7 +8292,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>439</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17.25" thickBot="1">
@@ -8293,7 +8300,7 @@
         <v>76</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17.25" thickBot="1">
@@ -8301,7 +8308,7 @@
         <v>77</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>441</v>
+        <v>376</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17.25" thickBot="1">
@@ -8309,7 +8316,7 @@
         <v>78</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>442</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17.25" thickBot="1">
@@ -8317,7 +8324,7 @@
         <v>79</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>443</v>
+        <v>378</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17.25" thickBot="1">
@@ -8325,7 +8332,7 @@
         <v>80</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>444</v>
+        <v>379</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17.25" thickBot="1">
@@ -8333,7 +8340,7 @@
         <v>81</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>445</v>
+        <v>380</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.25" thickBot="1">
@@ -8341,7 +8348,7 @@
         <v>82</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>446</v>
+        <v>381</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17.25" thickBot="1">
@@ -8349,7 +8356,7 @@
         <v>83</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>447</v>
+        <v>382</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17.25" thickBot="1">
@@ -8357,7 +8364,7 @@
         <v>84</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>448</v>
+        <v>383</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="17.25" thickBot="1">
@@ -8365,7 +8372,7 @@
         <v>85</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>449</v>
+        <v>384</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17.25" thickBot="1">
@@ -8373,7 +8380,7 @@
         <v>86</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>450</v>
+        <v>385</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="17.25" thickBot="1">
@@ -8381,7 +8388,7 @@
         <v>87</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>451</v>
+        <v>386</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17.25" thickBot="1">
@@ -8389,7 +8396,7 @@
         <v>88</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>452</v>
+        <v>387</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.25" thickBot="1">
@@ -8397,7 +8404,7 @@
         <v>89</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>453</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17.25" thickBot="1">
@@ -8405,7 +8412,7 @@
         <v>90</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>454</v>
+        <v>389</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17.25" thickBot="1">
@@ -8413,7 +8420,7 @@
         <v>91</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>455</v>
+        <v>390</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17.25" thickBot="1">
@@ -8421,7 +8428,7 @@
         <v>92</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>456</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17.25" thickBot="1">
@@ -8429,7 +8436,7 @@
         <v>93</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>457</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17.25" thickBot="1">
@@ -8437,7 +8444,7 @@
         <v>96</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>458</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17.25" thickBot="1">
@@ -8445,7 +8452,7 @@
         <v>97</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>459</v>
+        <v>394</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="17.25" thickBot="1">
@@ -8453,7 +8460,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>460</v>
+        <v>395</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17.25" thickBot="1">
@@ -8461,7 +8468,7 @@
         <v>99</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>461</v>
+        <v>396</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17.25" thickBot="1">
@@ -8469,7 +8476,7 @@
         <v>100</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>462</v>
+        <v>397</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17.25" thickBot="1">
@@ -8477,7 +8484,7 @@
         <v>101</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>463</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17.25" thickBot="1">
@@ -8485,7 +8492,7 @@
         <v>102</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>464</v>
+        <v>399</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17.25" thickBot="1">
@@ -8493,7 +8500,7 @@
         <v>103</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>465</v>
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17.25" thickBot="1">
@@ -8501,7 +8508,7 @@
         <v>104</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>466</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="17.25" thickBot="1">
@@ -8509,7 +8516,7 @@
         <v>105</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>467</v>
+        <v>402</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="17.25" thickBot="1">
@@ -8517,7 +8524,7 @@
         <v>106</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>468</v>
+        <v>403</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="17.25" thickBot="1">
@@ -8525,7 +8532,7 @@
         <v>107</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>469</v>
+        <v>404</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="17.25" thickBot="1">
@@ -8533,7 +8540,7 @@
         <v>108</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>470</v>
+        <v>405</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17.25" thickBot="1">
@@ -8541,7 +8548,7 @@
         <v>109</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>471</v>
+        <v>406</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17.25" thickBot="1">
@@ -8549,7 +8556,7 @@
         <v>110</v>
       </c>
       <c r="B82" s="37" t="s">
-        <v>472</v>
+        <v>407</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.25" thickBot="1">
@@ -8557,7 +8564,7 @@
         <v>111</v>
       </c>
       <c r="B83" s="37" t="s">
-        <v>473</v>
+        <v>408</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17.25" thickBot="1">
@@ -8565,7 +8572,7 @@
         <v>112</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>474</v>
+        <v>409</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="17.25" thickBot="1">
@@ -8573,7 +8580,7 @@
         <v>113</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>475</v>
+        <v>410</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17.25" thickBot="1">
@@ -8581,7 +8588,7 @@
         <v>114</v>
       </c>
       <c r="B86" s="37" t="s">
-        <v>476</v>
+        <v>411</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17.25" thickBot="1">
@@ -8589,7 +8596,7 @@
         <v>115</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>477</v>
+        <v>412</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17.25" thickBot="1">
@@ -8597,7 +8604,7 @@
         <v>116</v>
       </c>
       <c r="B88" s="37" t="s">
-        <v>478</v>
+        <v>413</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17.25" thickBot="1">
@@ -8605,7 +8612,7 @@
         <v>117</v>
       </c>
       <c r="B89" s="37" t="s">
-        <v>479</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17.25" thickBot="1">
@@ -8613,7 +8620,7 @@
         <v>118</v>
       </c>
       <c r="B90" s="37" t="s">
-        <v>480</v>
+        <v>415</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17.25" thickBot="1">
@@ -8621,7 +8628,7 @@
         <v>119</v>
       </c>
       <c r="B91" s="37" t="s">
-        <v>481</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="17.25" thickBot="1">
@@ -8629,7 +8636,7 @@
         <v>120</v>
       </c>
       <c r="B92" s="37" t="s">
-        <v>482</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="17.25" thickBot="1">
@@ -8637,7 +8644,7 @@
         <v>121</v>
       </c>
       <c r="B93" s="37" t="s">
-        <v>483</v>
+        <v>418</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="17.25" thickBot="1">
@@ -8645,7 +8652,7 @@
         <v>124</v>
       </c>
       <c r="B94" s="37" t="s">
-        <v>484</v>
+        <v>419</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="17.25" thickBot="1">
@@ -8653,7 +8660,7 @@
         <v>125</v>
       </c>
       <c r="B95" s="37" t="s">
-        <v>485</v>
+        <v>420</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="17.25" thickBot="1">
@@ -8661,7 +8668,7 @@
         <v>126</v>
       </c>
       <c r="B96" s="37" t="s">
-        <v>486</v>
+        <v>421</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="17.25" thickBot="1">
@@ -8669,7 +8676,7 @@
         <v>127</v>
       </c>
       <c r="B97" s="37" t="s">
-        <v>487</v>
+        <v>422</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="17.25" thickBot="1">
@@ -8677,7 +8684,7 @@
         <v>128</v>
       </c>
       <c r="B98" s="37" t="s">
-        <v>488</v>
+        <v>423</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="17.25" thickBot="1">
@@ -8685,7 +8692,7 @@
         <v>129</v>
       </c>
       <c r="B99" s="37" t="s">
-        <v>489</v>
+        <v>424</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17.25" thickBot="1">
@@ -8693,7 +8700,7 @@
         <v>130</v>
       </c>
       <c r="B100" s="37" t="s">
-        <v>490</v>
+        <v>425</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17.25" thickBot="1">
@@ -8701,7 +8708,7 @@
         <v>131</v>
       </c>
       <c r="B101" s="37" t="s">
-        <v>491</v>
+        <v>426</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.25" thickBot="1">
@@ -8709,7 +8716,7 @@
         <v>132</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>492</v>
+        <v>427</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17.25" thickBot="1">
@@ -8717,7 +8724,7 @@
         <v>133</v>
       </c>
       <c r="B103" s="37" t="s">
-        <v>493</v>
+        <v>428</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17.25" thickBot="1">
@@ -8725,7 +8732,7 @@
         <v>134</v>
       </c>
       <c r="B104" s="37" t="s">
-        <v>494</v>
+        <v>429</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17.25" thickBot="1">
@@ -8733,7 +8740,7 @@
         <v>135</v>
       </c>
       <c r="B105" s="37" t="s">
-        <v>495</v>
+        <v>430</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17.25" thickBot="1">
@@ -8741,7 +8748,7 @@
         <v>136</v>
       </c>
       <c r="B106" s="37" t="s">
-        <v>496</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="17.25" thickBot="1">
@@ -8749,7 +8756,7 @@
         <v>137</v>
       </c>
       <c r="B107" s="37" t="s">
-        <v>497</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="17.25" thickBot="1">
@@ -8757,7 +8764,7 @@
         <v>138</v>
       </c>
       <c r="B108" s="37" t="s">
-        <v>498</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="17.25" thickBot="1">
@@ -8765,7 +8772,7 @@
         <v>139</v>
       </c>
       <c r="B109" s="37" t="s">
-        <v>499</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17.25" thickBot="1">
@@ -8773,7 +8780,7 @@
         <v>140</v>
       </c>
       <c r="B110" s="37" t="s">
-        <v>500</v>
+        <v>435</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="17.25" thickBot="1">
@@ -8781,7 +8788,7 @@
         <v>141</v>
       </c>
       <c r="B111" s="37" t="s">
-        <v>501</v>
+        <v>436</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="17.25" thickBot="1">
@@ -8789,7 +8796,7 @@
         <v>142</v>
       </c>
       <c r="B112" s="37" t="s">
-        <v>502</v>
+        <v>437</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="17.25" thickBot="1">
@@ -8797,7 +8804,7 @@
         <v>143</v>
       </c>
       <c r="B113" s="37" t="s">
-        <v>503</v>
+        <v>438</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="17.25" thickBot="1">
@@ -8805,7 +8812,7 @@
         <v>144</v>
       </c>
       <c r="B114" s="37" t="s">
-        <v>504</v>
+        <v>439</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17.25" thickBot="1">
@@ -8813,7 +8820,7 @@
         <v>145</v>
       </c>
       <c r="B115" s="37" t="s">
-        <v>505</v>
+        <v>440</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17.25" thickBot="1">
@@ -8821,7 +8828,7 @@
         <v>146</v>
       </c>
       <c r="B116" s="37" t="s">
-        <v>506</v>
+        <v>441</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17.25" thickBot="1">
@@ -8829,7 +8836,7 @@
         <v>147</v>
       </c>
       <c r="B117" s="37" t="s">
-        <v>507</v>
+        <v>442</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="17.25" thickBot="1">
@@ -8837,7 +8844,7 @@
         <v>148</v>
       </c>
       <c r="B118" s="37" t="s">
-        <v>508</v>
+        <v>443</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="17.25" thickBot="1">
@@ -8845,7 +8852,7 @@
         <v>149</v>
       </c>
       <c r="B119" s="37" t="s">
-        <v>509</v>
+        <v>444</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="17.25" thickBot="1">
@@ -8853,7 +8860,7 @@
         <v>150</v>
       </c>
       <c r="B120" s="37" t="s">
-        <v>510</v>
+        <v>445</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="17.25" thickBot="1">
@@ -8861,7 +8868,7 @@
         <v>151</v>
       </c>
       <c r="B121" s="37" t="s">
-        <v>511</v>
+        <v>446</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="17.25" thickBot="1">
@@ -8869,7 +8876,7 @@
         <v>152</v>
       </c>
       <c r="B122" s="37" t="s">
-        <v>512</v>
+        <v>447</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="17.25" thickBot="1">
@@ -8877,7 +8884,7 @@
         <v>153</v>
       </c>
       <c r="B123" s="37" t="s">
-        <v>513</v>
+        <v>448</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="17.25" thickBot="1">
@@ -8885,7 +8892,7 @@
         <v>154</v>
       </c>
       <c r="B124" s="37" t="s">
-        <v>514</v>
+        <v>449</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="17.25" thickBot="1">
@@ -8893,7 +8900,7 @@
         <v>155</v>
       </c>
       <c r="B125" s="37" t="s">
-        <v>515</v>
+        <v>450</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="17.25" thickBot="1">
@@ -8901,15 +8908,15 @@
         <v>156</v>
       </c>
       <c r="B126" s="37" t="s">
-        <v>516</v>
+        <v>451</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="17.25" thickBot="1">
       <c r="A127" s="36" t="s">
-        <v>383</v>
+        <v>318</v>
       </c>
       <c r="B127" s="37" t="s">
-        <v>517</v>
+        <v>452</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="17.25" thickBot="1">
@@ -8917,7 +8924,7 @@
         <v>68</v>
       </c>
       <c r="B128" s="37" t="s">
-        <v>518</v>
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="17.25" thickBot="1">
@@ -8925,7 +8932,7 @@
         <v>69</v>
       </c>
       <c r="B129" s="37" t="s">
-        <v>519</v>
+        <v>454</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="17.25" thickBot="1">
@@ -8941,7 +8948,7 @@
         <v>57</v>
       </c>
       <c r="B131" s="37" t="s">
-        <v>520</v>
+        <v>455</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="17.25" thickBot="1">
@@ -8952,10 +8959,10 @@
     </row>
     <row r="133" spans="1:2" ht="17.25" thickBot="1">
       <c r="A133" s="36" t="s">
-        <v>521</v>
+        <v>456</v>
       </c>
       <c r="B133" s="37" t="s">
-        <v>520</v>
+        <v>455</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="16.5">
@@ -8976,7 +8983,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="Z16:BH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="BH45" sqref="BH45"/>
     </sheetView>
   </sheetViews>
@@ -8984,46 +8991,46 @@
   <sheetData>
     <row r="16" spans="35:60" ht="12.75" customHeight="1">
       <c r="AI16" s="47" t="s">
-        <v>526</v>
+        <v>461</v>
       </c>
       <c r="BH16" s="47" t="s">
-        <v>526</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="26:51" ht="12.75" customHeight="1">
       <c r="Z22" s="47" t="s">
-        <v>525</v>
+        <v>460</v>
       </c>
       <c r="AY22" s="47" t="s">
-        <v>525</v>
+        <v>460</v>
       </c>
     </row>
     <row r="54" spans="26:51" ht="12.75" customHeight="1">
       <c r="AY54" s="47" t="s">
-        <v>526</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58" spans="26:51" ht="12.75" customHeight="1">
       <c r="AI58" s="47" t="s">
-        <v>526</v>
+        <v>461</v>
       </c>
     </row>
     <row r="64" spans="26:51" ht="12.75" customHeight="1">
       <c r="Z64" s="47" t="s">
-        <v>525</v>
+        <v>460</v>
       </c>
       <c r="AY64" s="47" t="s">
-        <v>525</v>
+        <v>460</v>
       </c>
     </row>
     <row r="86" spans="51:60" ht="12.75" customHeight="1">
       <c r="BH86" s="47" t="s">
-        <v>526</v>
+        <v>461</v>
       </c>
     </row>
     <row r="92" spans="51:60" ht="12.75" customHeight="1">
       <c r="AY92" s="47" t="s">
-        <v>525</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pin definition for QT600 interface board debug interface.
Added SPI bit bang Data Interface pins for interfacing with the
QT600 Interface Board to use with QTouch Studio for debugging.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="535">
   <si>
     <t>PIN</t>
   </si>
@@ -1603,6 +1603,27 @@
   </si>
   <si>
     <t>??? Perhaps use for USB firmware upgrade ???</t>
+  </si>
+  <si>
+    <t>QT_DEBUG_INTERFACE</t>
+  </si>
+  <si>
+    <t>SS_BB</t>
+  </si>
+  <si>
+    <t>SCK_BB</t>
+  </si>
+  <si>
+    <t>MOSI_BB</t>
+  </si>
+  <si>
+    <t>MISO_BB</t>
+  </si>
+  <si>
+    <t>Debug Interface for QT600</t>
+  </si>
+  <si>
+    <t>Comes out to suitable header for Target Data on QT600 interface board</t>
   </si>
 </sst>
 </file>
@@ -2153,6 +2174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2162,7 +2184,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4208,8 +4229,8 @@
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J136" sqref="J136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4225,21 +4246,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickTop="1" thickBot="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="45" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="44" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="45"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:10" s="43" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="40" t="s">
@@ -7388,16 +7409,20 @@
       </c>
       <c r="C132" s="31"/>
       <c r="D132" s="31" t="s">
-        <v>238</v>
+        <v>529</v>
       </c>
       <c r="E132" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="F132" s="31"/>
+        <v>528</v>
+      </c>
+      <c r="F132" s="31" t="s">
+        <v>533</v>
+      </c>
       <c r="G132" s="31"/>
       <c r="H132" s="31"/>
       <c r="I132" s="32"/>
-      <c r="J132" s="33"/>
+      <c r="J132" s="33" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="30">
@@ -7408,16 +7433,20 @@
       </c>
       <c r="C133" s="31"/>
       <c r="D133" s="31" t="s">
-        <v>238</v>
+        <v>530</v>
       </c>
       <c r="E133" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="F133" s="31"/>
+        <v>528</v>
+      </c>
+      <c r="F133" s="31" t="s">
+        <v>533</v>
+      </c>
       <c r="G133" s="31"/>
       <c r="H133" s="31"/>
       <c r="I133" s="32"/>
-      <c r="J133" s="33"/>
+      <c r="J133" s="33" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134" s="30">
@@ -7428,16 +7457,20 @@
       </c>
       <c r="C134" s="31"/>
       <c r="D134" s="31" t="s">
-        <v>238</v>
+        <v>531</v>
       </c>
       <c r="E134" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="F134" s="31"/>
+        <v>528</v>
+      </c>
+      <c r="F134" s="31" t="s">
+        <v>533</v>
+      </c>
       <c r="G134" s="31"/>
       <c r="H134" s="31"/>
       <c r="I134" s="32"/>
-      <c r="J134" s="33"/>
+      <c r="J134" s="33" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="30">
@@ -7448,16 +7481,20 @@
       </c>
       <c r="C135" s="31"/>
       <c r="D135" s="31" t="s">
-        <v>238</v>
+        <v>532</v>
       </c>
       <c r="E135" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="F135" s="31"/>
+        <v>528</v>
+      </c>
+      <c r="F135" s="31" t="s">
+        <v>533</v>
+      </c>
       <c r="G135" s="31"/>
       <c r="H135" s="31"/>
       <c r="I135" s="32"/>
-      <c r="J135" s="33"/>
+      <c r="J135" s="33" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="30">
@@ -8990,46 +9027,46 @@
   <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="12.75" customHeight="1"/>
   <sheetData>
     <row r="16" spans="35:60" ht="12.75" customHeight="1">
-      <c r="AI16" s="47" t="s">
+      <c r="AI16" s="44" t="s">
         <v>461</v>
       </c>
-      <c r="BH16" s="47" t="s">
+      <c r="BH16" s="44" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="22" spans="26:51" ht="12.75" customHeight="1">
-      <c r="Z22" s="47" t="s">
+      <c r="Z22" s="44" t="s">
         <v>460</v>
       </c>
-      <c r="AY22" s="47" t="s">
+      <c r="AY22" s="44" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="54" spans="26:51" ht="12.75" customHeight="1">
-      <c r="AY54" s="47" t="s">
+      <c r="AY54" s="44" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="58" spans="26:51" ht="12.75" customHeight="1">
-      <c r="AI58" s="47" t="s">
+      <c r="AI58" s="44" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="64" spans="26:51" ht="12.75" customHeight="1">
-      <c r="Z64" s="47" t="s">
+      <c r="Z64" s="44" t="s">
         <v>460</v>
       </c>
-      <c r="AY64" s="47" t="s">
+      <c r="AY64" s="44" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="86" spans="51:60" ht="12.75" customHeight="1">
-      <c r="BH86" s="47" t="s">
+      <c r="BH86" s="44" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="92" spans="51:60" ht="12.75" customHeight="1">
-      <c r="AY92" s="47" t="s">
+      <c r="AY92" s="44" t="s">
         <v>460</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Further board updates and pin changes.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -4224,13 +4224,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J136" sqref="J136"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4294,7 +4294,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickTop="1">
+    <row r="3" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -4338,7 +4338,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="20"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -4360,7 +4360,7 @@
       <c r="I5" s="19"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="I6" s="19"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="15.75" thickTop="1">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11" s="13">
         <v>9</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1">
       <c r="A12" s="13">
         <v>10</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13" s="13">
         <v>11</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14" s="13">
         <v>12</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1">
       <c r="A16" s="13">
         <v>14</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" hidden="1">
       <c r="A17" s="13">
         <v>15</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18" s="13">
         <v>16</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19" s="13">
         <v>17</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20" s="13">
         <v>18</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21" s="13">
         <v>19</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="13">
         <v>20</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="13">
         <v>21</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24" s="13">
         <v>22</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="13">
         <v>23</v>
       </c>
@@ -4844,7 +4844,7 @@
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" s="13">
         <v>24</v>
       </c>
@@ -4866,7 +4866,7 @@
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="13">
         <v>25</v>
       </c>
@@ -4888,7 +4888,7 @@
       <c r="I27" s="19"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" s="13">
         <v>26</v>
       </c>
@@ -4910,7 +4910,7 @@
       <c r="I28" s="19"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29" s="13">
         <v>27</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="I29" s="19"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" s="13">
         <v>28</v>
       </c>
@@ -4954,7 +4954,7 @@
       <c r="I30" s="19"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31" s="13">
         <v>29</v>
       </c>
@@ -4976,7 +4976,7 @@
       <c r="I31" s="19"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="13">
         <v>30</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="I32" s="19"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="13">
         <v>31</v>
       </c>
@@ -5020,7 +5020,7 @@
       <c r="I33" s="19"/>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="13">
         <v>32</v>
       </c>
@@ -5042,7 +5042,7 @@
       <c r="I34" s="19"/>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35" s="13">
         <v>33</v>
       </c>
@@ -5064,7 +5064,7 @@
       <c r="I35" s="19"/>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36" s="13">
         <v>34</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37" s="13">
         <v>35</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38" s="13">
         <v>36</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41" s="22">
         <v>39</v>
       </c>
@@ -5212,7 +5212,7 @@
       <c r="I41" s="25"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1">
       <c r="A42" s="22">
         <v>40</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="I42" s="25"/>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43" s="22">
         <v>41</v>
       </c>
@@ -5256,7 +5256,7 @@
       <c r="I43" s="25"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1">
       <c r="A44" s="22">
         <v>42</v>
       </c>
@@ -5278,7 +5278,7 @@
       <c r="I44" s="25"/>
       <c r="J44" s="24"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45" s="22">
         <v>43</v>
       </c>
@@ -5300,7 +5300,7 @@
       <c r="I45" s="25"/>
       <c r="J45" s="24"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="22">
         <v>44</v>
       </c>
@@ -5322,7 +5322,7 @@
       <c r="I46" s="25"/>
       <c r="J46" s="24"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" s="22">
         <v>45</v>
       </c>
@@ -5344,7 +5344,7 @@
       <c r="I47" s="25"/>
       <c r="J47" s="24"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48" s="22">
         <v>46</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="I48" s="25"/>
       <c r="J48" s="24"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="22">
         <v>47</v>
       </c>
@@ -5388,7 +5388,7 @@
       <c r="I49" s="25"/>
       <c r="J49" s="24"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50" s="22">
         <v>48</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="22">
         <v>50</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="22">
         <v>51</v>
       </c>
@@ -5620,7 +5620,7 @@
       </c>
       <c r="J58" s="24"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="22">
         <v>57</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" s="22">
         <v>58</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="22">
         <v>59</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62" s="22">
         <v>60</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63" s="22">
         <v>61</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" hidden="1">
       <c r="A64" s="22">
         <v>62</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" hidden="1">
       <c r="A65" s="22">
         <v>63</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" hidden="1">
       <c r="A66" s="22">
         <v>64</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" hidden="1">
       <c r="A67" s="22">
         <v>65</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" hidden="1">
       <c r="A68" s="22">
         <v>66</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" hidden="1">
       <c r="A69" s="22">
         <v>67</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" hidden="1">
       <c r="A70" s="22">
         <v>68</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71" s="22">
         <v>69</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72" s="22">
         <v>70</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" hidden="1">
       <c r="A73" s="22">
         <v>71</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" hidden="1">
       <c r="A74" s="22">
         <v>72</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" hidden="1">
       <c r="A75" s="26">
         <v>73</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" hidden="1">
       <c r="A76" s="26">
         <v>74</v>
       </c>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="J78" s="29"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" hidden="1">
       <c r="A79" s="26">
         <v>77</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80" s="26">
         <v>78</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" hidden="1">
       <c r="A81" s="26">
         <v>79</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" hidden="1">
       <c r="A82" s="26">
         <v>80</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" hidden="1">
       <c r="A83" s="26">
         <v>81</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" hidden="1">
       <c r="A84" s="26">
         <v>82</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" hidden="1">
       <c r="A85" s="26">
         <v>83</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" hidden="1">
       <c r="A86" s="26">
         <v>84</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" hidden="1">
       <c r="A87" s="26">
         <v>85</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" hidden="1">
       <c r="A88" s="26">
         <v>86</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" hidden="1">
       <c r="A89" s="26">
         <v>87</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" hidden="1">
       <c r="A90" s="26">
         <v>88</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" hidden="1">
       <c r="A91" s="26">
         <v>89</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" hidden="1">
       <c r="A92" s="26">
         <v>90</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" hidden="1">
       <c r="A93" s="26">
         <v>91</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" hidden="1">
       <c r="A94" s="26">
         <v>92</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" hidden="1">
       <c r="A95" s="26">
         <v>93</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" hidden="1">
       <c r="A96" s="26">
         <v>94</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1">
       <c r="A97" s="26">
         <v>95</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98" s="26">
         <v>96</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" hidden="1">
       <c r="A99" s="26">
         <v>97</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" hidden="1">
       <c r="A100" s="26">
         <v>98</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" hidden="1">
       <c r="A101" s="26">
         <v>99</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" hidden="1">
       <c r="A102" s="26">
         <v>100</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" hidden="1">
       <c r="A103" s="26">
         <v>101</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" hidden="1">
       <c r="A104" s="26">
         <v>102</v>
       </c>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="J106" s="29"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" hidden="1">
       <c r="A107" s="26">
         <v>105</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" hidden="1">
       <c r="A108" s="26">
         <v>106</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" hidden="1">
       <c r="A109" s="26">
         <v>107</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="J109" s="29"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" hidden="1">
       <c r="A110" s="26">
         <v>108</v>
       </c>
@@ -6892,7 +6892,7 @@
       </c>
       <c r="J110" s="29"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" hidden="1">
       <c r="A111" s="30">
         <v>109</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" hidden="1">
       <c r="A112" s="30">
         <v>110</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" hidden="1">
       <c r="A113" s="30">
         <v>111</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" hidden="1">
       <c r="A114" s="30">
         <v>112</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" hidden="1">
       <c r="A115" s="30">
         <v>113</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" hidden="1">
       <c r="A116" s="30">
         <v>114</v>
       </c>
@@ -7064,7 +7064,7 @@
       <c r="I116" s="32"/>
       <c r="J116" s="33"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" hidden="1">
       <c r="A117" s="30">
         <v>115</v>
       </c>
@@ -7084,7 +7084,7 @@
       <c r="I117" s="32"/>
       <c r="J117" s="33"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" hidden="1">
       <c r="A118" s="30">
         <v>116</v>
       </c>
@@ -7104,7 +7104,7 @@
       <c r="I118" s="32"/>
       <c r="J118" s="33"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" hidden="1">
       <c r="A119" s="30">
         <v>117</v>
       </c>
@@ -7180,7 +7180,7 @@
       </c>
       <c r="J121" s="33"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" hidden="1">
       <c r="A122" s="30">
         <v>120</v>
       </c>
@@ -7202,7 +7202,7 @@
       <c r="I122" s="32"/>
       <c r="J122" s="33"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" hidden="1">
       <c r="A123" s="30">
         <v>121</v>
       </c>
@@ -7224,7 +7224,7 @@
       <c r="I123" s="32"/>
       <c r="J123" s="33"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" hidden="1">
       <c r="A124" s="30">
         <v>122</v>
       </c>
@@ -7246,7 +7246,7 @@
       <c r="I124" s="32"/>
       <c r="J124" s="33"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" hidden="1">
       <c r="A125" s="30">
         <v>123</v>
       </c>
@@ -7268,7 +7268,7 @@
       <c r="I125" s="32"/>
       <c r="J125" s="33"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" hidden="1">
       <c r="A126" s="30">
         <v>124</v>
       </c>
@@ -7290,7 +7290,7 @@
       <c r="I126" s="32"/>
       <c r="J126" s="33"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" hidden="1">
       <c r="A127" s="30">
         <v>125</v>
       </c>
@@ -7312,7 +7312,7 @@
       <c r="I127" s="32"/>
       <c r="J127" s="33"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" hidden="1">
       <c r="A128" s="30">
         <v>126</v>
       </c>
@@ -7334,7 +7334,7 @@
       <c r="I128" s="32"/>
       <c r="J128" s="33"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" hidden="1">
       <c r="A129" s="30">
         <v>127</v>
       </c>
@@ -7356,7 +7356,7 @@
       <c r="I129" s="32"/>
       <c r="J129" s="33"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" hidden="1">
       <c r="A130" s="30">
         <v>128</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="I130" s="32"/>
       <c r="J130" s="33"/>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" hidden="1">
       <c r="A131" s="30">
         <v>129</v>
       </c>
@@ -7400,7 +7400,7 @@
       <c r="I131" s="32"/>
       <c r="J131" s="33"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" hidden="1">
       <c r="A132" s="30">
         <v>130</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" hidden="1">
       <c r="A133" s="30">
         <v>131</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" hidden="1">
       <c r="A134" s="30">
         <v>132</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" hidden="1">
       <c r="A135" s="30">
         <v>133</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" hidden="1">
       <c r="A136" s="30">
         <v>134</v>
       </c>
@@ -7516,7 +7516,7 @@
       <c r="I136" s="32"/>
       <c r="J136" s="33"/>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" hidden="1">
       <c r="A137" s="30">
         <v>135</v>
       </c>
@@ -7536,7 +7536,7 @@
       <c r="I137" s="32"/>
       <c r="J137" s="33"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" hidden="1">
       <c r="A138" s="30">
         <v>136</v>
       </c>
@@ -7556,7 +7556,7 @@
       <c r="I138" s="32"/>
       <c r="J138" s="33"/>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" hidden="1">
       <c r="A139" s="30">
         <v>137</v>
       </c>
@@ -7576,7 +7576,7 @@
       <c r="I139" s="32"/>
       <c r="J139" s="33"/>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" hidden="1">
       <c r="A140" s="30">
         <v>138</v>
       </c>
@@ -7596,7 +7596,7 @@
       <c r="I140" s="32"/>
       <c r="J140" s="33"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" hidden="1">
       <c r="A141" s="30">
         <v>139</v>
       </c>
@@ -7616,7 +7616,7 @@
       <c r="I141" s="32"/>
       <c r="J141" s="33"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" hidden="1">
       <c r="A142" s="30">
         <v>140</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" hidden="1">
       <c r="A143" s="30">
         <v>141</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" hidden="1">
       <c r="A144" s="30">
         <v>142</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" hidden="1">
       <c r="A145" s="30">
         <v>143</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" hidden="1">
       <c r="A146" s="30">
         <v>144</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" hidden="1">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -7760,7 +7760,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" hidden="1">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -7784,7 +7784,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" hidden="1">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -7808,7 +7808,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" hidden="1">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -7832,7 +7832,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" hidden="1">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -7856,7 +7856,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" hidden="1">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -7880,7 +7880,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="15.75" thickBot="1">
+    <row r="153" spans="1:10" ht="15.75" hidden="1" thickBot="1">
       <c r="A153" s="6"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -7902,7 +7902,6 @@
         <v>320</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="15.75" thickTop="1"/>
     <row r="155" spans="1:10">
       <c r="A155" s="10" t="s">
         <v>322</v>
@@ -7911,7 +7910,11 @@
   </sheetData>
   <autoFilter ref="A2:J153">
     <filterColumn colId="2"/>
-    <filterColumn colId="4"/>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="SUPPLY"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="6"/>
     <filterColumn colId="8"/>
   </autoFilter>

</xml_diff>

<commit_message>
Updated the Pin Assignment file.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -4382,7 +4382,7 @@
       <c r="I6" s="19"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickTop="1">
+    <row r="7" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:10" hidden="1">
+    <row r="9" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1">
+    <row r="10" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1">
+    <row r="11" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A11" s="13">
         <v>9</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1">
+    <row r="12" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A12" s="13">
         <v>10</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1">
+    <row r="13" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A13" s="13">
         <v>11</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1">
+    <row r="14" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A14" s="13">
         <v>12</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1">
+    <row r="15" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A16" s="13">
         <v>14</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1">
+    <row r="17" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A17" s="13">
         <v>15</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1">
+    <row r="18" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A18" s="13">
         <v>16</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1">
+    <row r="19" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A19" s="13">
         <v>17</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1">
+    <row r="20" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A20" s="13">
         <v>18</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1">
+    <row r="21" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A21" s="13">
         <v>19</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1">
+    <row r="22" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A22" s="13">
         <v>20</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1">
+    <row r="23" spans="1:10" ht="15.75" hidden="1" thickTop="1">
       <c r="A23" s="13">
         <v>21</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1">
+    <row r="24" spans="1:10" ht="15.75" thickTop="1">
       <c r="A24" s="13">
         <v>22</v>
       </c>
@@ -5130,7 +5130,7 @@
       <c r="I38" s="19"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39" s="22">
         <v>37</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1">
       <c r="A40" s="22">
         <v>38</v>
       </c>
@@ -5410,7 +5410,7 @@
       <c r="I50" s="25"/>
       <c r="J50" s="24"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="22">
         <v>49</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="22">
         <v>52</v>
       </c>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="J54" s="24"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55" s="22">
         <v>53</v>
       </c>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="J55" s="24"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="22">
         <v>54</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="22">
         <v>55</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" hidden="1">
       <c r="A58" s="22">
         <v>56</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" hidden="1">
       <c r="A77" s="26">
         <v>75</v>
       </c>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="J77" s="29"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" hidden="1">
       <c r="A78" s="26">
         <v>76</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" hidden="1">
       <c r="A105" s="26">
         <v>103</v>
       </c>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="J105" s="29"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" hidden="1">
       <c r="A106" s="26">
         <v>104</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1">
+    <row r="109" spans="1:10">
       <c r="A109" s="26">
         <v>107</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="J109" s="29"/>
     </row>
-    <row r="110" spans="1:10" hidden="1">
+    <row r="110" spans="1:10">
       <c r="A110" s="26">
         <v>108</v>
       </c>
@@ -6892,7 +6892,7 @@
       </c>
       <c r="J110" s="29"/>
     </row>
-    <row r="111" spans="1:10" hidden="1">
+    <row r="111" spans="1:10">
       <c r="A111" s="30">
         <v>109</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1">
+    <row r="112" spans="1:10">
       <c r="A112" s="30">
         <v>110</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1">
+    <row r="113" spans="1:10">
       <c r="A113" s="30">
         <v>111</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1">
+    <row r="114" spans="1:10">
       <c r="A114" s="30">
         <v>112</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1">
+    <row r="115" spans="1:10">
       <c r="A115" s="30">
         <v>113</v>
       </c>
@@ -7124,7 +7124,7 @@
       <c r="I119" s="32"/>
       <c r="J119" s="33"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" hidden="1">
       <c r="A120" s="30">
         <v>118</v>
       </c>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="J120" s="33"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" hidden="1">
       <c r="A121" s="30">
         <v>119</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1">
+    <row r="147" spans="1:10">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -7760,7 +7760,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1">
+    <row r="148" spans="1:10">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -7784,7 +7784,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1">
+    <row r="149" spans="1:10">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -7808,7 +7808,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1">
+    <row r="150" spans="1:10">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -7832,7 +7832,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1">
+    <row r="151" spans="1:10">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -7856,7 +7856,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1">
+    <row r="152" spans="1:10">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -7912,7 +7912,7 @@
     <filterColumn colId="2"/>
     <filterColumn colId="4">
       <filters>
-        <filter val="SUPPLY"/>
+        <filter val="SHIELD-DATA-TRANSFER"/>
       </filters>
     </filterColumn>
     <filterColumn colId="6"/>

</xml_diff>

<commit_message>
Added full list of STK600 pins to AVR32 MCU pinning list.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="535">
   <si>
     <t>PIN</t>
   </si>
@@ -1712,7 +1712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -2039,11 +2039,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2182,6 +2195,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4224,19 +4240,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1" filterMode="1">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4294,14 +4311,17 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="3" spans="1:10" ht="15.75" thickTop="1">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="15" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B3),VLOOKUP(B3,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA0, TCK</v>
+      </c>
       <c r="D3" s="14" t="s">
         <v>9</v>
       </c>
@@ -4316,14 +4336,17 @@
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="4" spans="1:10">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="48" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B4),VLOOKUP(B4,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA1, TDI</v>
+      </c>
       <c r="D4" s="18" t="s">
         <v>10</v>
       </c>
@@ -4338,14 +4361,17 @@
       <c r="I4" s="19"/>
       <c r="J4" s="20"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="5" spans="1:10">
       <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B5),VLOOKUP(B5,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA2, TDO</v>
+      </c>
       <c r="D5" s="18" t="s">
         <v>11</v>
       </c>
@@ -4360,14 +4386,17 @@
       <c r="I5" s="19"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="6" spans="1:10">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B6),VLOOKUP(B6,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA3, TMS</v>
+      </c>
       <c r="D6" s="18" t="s">
         <v>12</v>
       </c>
@@ -4382,14 +4411,17 @@
       <c r="I6" s="19"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="7" spans="1:10">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B7),VLOOKUP(B7,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
@@ -4410,14 +4442,17 @@
       </c>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="8" spans="1:10">
       <c r="A8" s="13">
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B8),VLOOKUP(B8,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D8" s="18" t="s">
         <v>17</v>
       </c>
@@ -4438,14 +4473,17 @@
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="9" spans="1:10">
       <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B9),VLOOKUP(B9,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE4</v>
+      </c>
       <c r="D9" s="18" t="s">
         <v>166</v>
       </c>
@@ -4462,14 +4500,17 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="10" spans="1:10">
       <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B10),VLOOKUP(B10,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE5</v>
+      </c>
       <c r="D10" s="18" t="s">
         <v>167</v>
       </c>
@@ -4486,14 +4527,17 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="11" spans="1:10">
       <c r="A11" s="13">
         <v>9</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B11),VLOOKUP(B11,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE6</v>
+      </c>
       <c r="D11" s="18" t="s">
         <v>168</v>
       </c>
@@ -4510,14 +4554,17 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="12" spans="1:10">
       <c r="A12" s="13">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B12),VLOOKUP(B12,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE7</v>
+      </c>
       <c r="D12" s="18" t="s">
         <v>169</v>
       </c>
@@ -4534,14 +4581,17 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="13" spans="1:10">
       <c r="A13" s="13">
         <v>11</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B13),VLOOKUP(B13,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF0</v>
+      </c>
       <c r="D13" s="18" t="s">
         <v>170</v>
       </c>
@@ -4558,14 +4608,17 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="14" spans="1:10">
       <c r="A14" s="13">
         <v>12</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B14),VLOOKUP(B14,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF1</v>
+      </c>
       <c r="D14" s="18" t="s">
         <v>171</v>
       </c>
@@ -4582,14 +4635,17 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="15" spans="1:10">
       <c r="A15" s="13">
         <v>13</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B15),VLOOKUP(B15,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF2</v>
+      </c>
       <c r="D15" s="18" t="s">
         <v>45</v>
       </c>
@@ -4606,14 +4662,17 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="16" spans="1:10">
       <c r="A16" s="13">
         <v>14</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B16),VLOOKUP(B16,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF3</v>
+      </c>
       <c r="D16" s="18" t="s">
         <v>46</v>
       </c>
@@ -4630,14 +4689,17 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="17" spans="1:10">
       <c r="A17" s="13">
         <v>15</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B17),VLOOKUP(B17,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF4</v>
+      </c>
       <c r="D17" s="18" t="s">
         <v>47</v>
       </c>
@@ -4654,14 +4716,17 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="18" spans="1:10">
       <c r="A18" s="13">
         <v>16</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B18),VLOOKUP(B18,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF5</v>
+      </c>
       <c r="D18" s="18" t="s">
         <v>48</v>
       </c>
@@ -4678,14 +4743,17 @@
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="19" spans="1:10">
       <c r="A19" s="13">
         <v>17</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B19),VLOOKUP(B19,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF6</v>
+      </c>
       <c r="D19" s="18" t="s">
         <v>49</v>
       </c>
@@ -4702,14 +4770,17 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="20" spans="1:10">
       <c r="A20" s="13">
         <v>18</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B20),VLOOKUP(B20,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PF7</v>
+      </c>
       <c r="D20" s="18" t="s">
         <v>50</v>
       </c>
@@ -4726,14 +4797,17 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="13">
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B21),VLOOKUP(B21,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG0</v>
+      </c>
       <c r="D21" s="18" t="s">
         <v>51</v>
       </c>
@@ -4750,14 +4824,17 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="22" spans="1:10">
       <c r="A22" s="13">
         <v>20</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B22),VLOOKUP(B22,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG1</v>
+      </c>
       <c r="D22" s="18" t="s">
         <v>52</v>
       </c>
@@ -4774,14 +4851,17 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" hidden="1" thickTop="1">
+    <row r="23" spans="1:10">
       <c r="A23" s="13">
         <v>21</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B23),VLOOKUP(B23,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA4</v>
+      </c>
       <c r="D23" s="18" t="s">
         <v>241</v>
       </c>
@@ -4798,14 +4878,17 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickTop="1">
+    <row r="24" spans="1:10">
       <c r="A24" s="13">
         <v>22</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="18"/>
+      <c r="C24" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B24),VLOOKUP(B24,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA5</v>
+      </c>
       <c r="D24" s="18" t="s">
         <v>242</v>
       </c>
@@ -4822,14 +4905,17 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1">
+    <row r="25" spans="1:10">
       <c r="A25" s="13">
         <v>23</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B25),VLOOKUP(B25,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA6</v>
+      </c>
       <c r="D25" s="18" t="s">
         <v>463</v>
       </c>
@@ -4844,14 +4930,17 @@
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:10">
       <c r="A26" s="13">
         <v>24</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="18"/>
+      <c r="C26" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B26),VLOOKUP(B26,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PA7</v>
+      </c>
       <c r="D26" s="18" t="s">
         <v>464</v>
       </c>
@@ -4866,14 +4955,17 @@
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" hidden="1">
+    <row r="27" spans="1:10">
       <c r="A27" s="13">
         <v>25</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B27),VLOOKUP(B27,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB0</v>
+      </c>
       <c r="D27" s="18" t="s">
         <v>465</v>
       </c>
@@ -4888,14 +4980,17 @@
       <c r="I27" s="19"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" hidden="1">
+    <row r="28" spans="1:10">
       <c r="A28" s="13">
         <v>26</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B28),VLOOKUP(B28,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB1</v>
+      </c>
       <c r="D28" s="18" t="s">
         <v>466</v>
       </c>
@@ -4910,14 +5005,17 @@
       <c r="I28" s="19"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="13">
         <v>27</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="18"/>
+      <c r="C29" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B29),VLOOKUP(B29,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB2</v>
+      </c>
       <c r="D29" s="18" t="s">
         <v>467</v>
       </c>
@@ -4932,14 +5030,17 @@
       <c r="I29" s="19"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" hidden="1">
+    <row r="30" spans="1:10">
       <c r="A30" s="13">
         <v>28</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B30),VLOOKUP(B30,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB3, AREF1</v>
+      </c>
       <c r="D30" s="18" t="s">
         <v>468</v>
       </c>
@@ -4954,14 +5055,17 @@
       <c r="I30" s="19"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" hidden="1">
+    <row r="31" spans="1:10">
       <c r="A31" s="13">
         <v>29</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="18"/>
+      <c r="C31" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B31),VLOOKUP(B31,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB4</v>
+      </c>
       <c r="D31" s="18" t="s">
         <v>469</v>
       </c>
@@ -4976,14 +5080,17 @@
       <c r="I31" s="19"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:10">
       <c r="A32" s="13">
         <v>30</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B32),VLOOKUP(B32,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB5</v>
+      </c>
       <c r="D32" s="18" t="s">
         <v>470</v>
       </c>
@@ -4998,14 +5105,17 @@
       <c r="I32" s="19"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:10" hidden="1">
+    <row r="33" spans="1:10">
       <c r="A33" s="13">
         <v>31</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="18"/>
+      <c r="C33" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B33),VLOOKUP(B33,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB6</v>
+      </c>
       <c r="D33" s="18" t="s">
         <v>471</v>
       </c>
@@ -5020,14 +5130,17 @@
       <c r="I33" s="19"/>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10">
       <c r="A34" s="13">
         <v>32</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B34),VLOOKUP(B34,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PB7</v>
+      </c>
       <c r="D34" s="18" t="s">
         <v>472</v>
       </c>
@@ -5042,14 +5155,17 @@
       <c r="I34" s="19"/>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="1:10" hidden="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="13">
         <v>33</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B35),VLOOKUP(B35,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC0, AREF0</v>
+      </c>
       <c r="D35" s="18" t="s">
         <v>473</v>
       </c>
@@ -5064,14 +5180,17 @@
       <c r="I35" s="19"/>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10" hidden="1">
+    <row r="36" spans="1:10">
       <c r="A36" s="13">
         <v>34</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B36),VLOOKUP(B36,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D36" s="18" t="s">
         <v>238</v>
       </c>
@@ -5086,14 +5205,17 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1">
+    <row r="37" spans="1:10">
       <c r="A37" s="13">
         <v>35</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="18"/>
+      <c r="C37" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B37),VLOOKUP(B37,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D37" s="18" t="s">
         <v>238</v>
       </c>
@@ -5108,14 +5230,17 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1">
+    <row r="38" spans="1:10">
       <c r="A38" s="13">
         <v>36</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="18"/>
+      <c r="C38" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B38),VLOOKUP(B38,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC3</v>
+      </c>
       <c r="D38" s="18" t="s">
         <v>474</v>
       </c>
@@ -5130,14 +5255,17 @@
       <c r="I38" s="19"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10" hidden="1">
+    <row r="39" spans="1:10">
       <c r="A39" s="22">
         <v>37</v>
       </c>
       <c r="B39" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="23"/>
+      <c r="C39" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B39),VLOOKUP(B39,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D39" s="23" t="s">
         <v>17</v>
       </c>
@@ -5160,14 +5288,17 @@
         <v>282</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1">
+    <row r="40" spans="1:10">
       <c r="A40" s="22">
         <v>38</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="23"/>
+      <c r="C40" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B40),VLOOKUP(B40,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>VTG</v>
+      </c>
       <c r="D40" s="23" t="s">
         <v>15</v>
       </c>
@@ -5190,14 +5321,17 @@
         <v>281</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1">
+    <row r="41" spans="1:10">
       <c r="A41" s="22">
         <v>39</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="23"/>
+      <c r="C41" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B41),VLOOKUP(B41,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC4</v>
+      </c>
       <c r="D41" s="23" t="s">
         <v>475</v>
       </c>
@@ -5212,14 +5346,17 @@
       <c r="I41" s="25"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:10" hidden="1">
+    <row r="42" spans="1:10">
       <c r="A42" s="22">
         <v>40</v>
       </c>
       <c r="B42" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="23"/>
+      <c r="C42" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B42),VLOOKUP(B42,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC5</v>
+      </c>
       <c r="D42" s="23" t="s">
         <v>476</v>
       </c>
@@ -5234,14 +5371,17 @@
       <c r="I42" s="25"/>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10" hidden="1">
+    <row r="43" spans="1:10">
       <c r="A43" s="22">
         <v>41</v>
       </c>
       <c r="B43" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="23"/>
+      <c r="C43" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B43),VLOOKUP(B43,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC6</v>
+      </c>
       <c r="D43" s="23" t="s">
         <v>477</v>
       </c>
@@ -5256,14 +5396,17 @@
       <c r="I43" s="25"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="22">
         <v>42</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="23"/>
+      <c r="C44" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B44),VLOOKUP(B44,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PC7</v>
+      </c>
       <c r="D44" s="23" t="s">
         <v>478</v>
       </c>
@@ -5278,14 +5421,17 @@
       <c r="I44" s="25"/>
       <c r="J44" s="24"/>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="22">
         <v>43</v>
       </c>
       <c r="B45" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="23"/>
+      <c r="C45" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B45),VLOOKUP(B45,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD0</v>
+      </c>
       <c r="D45" s="23" t="s">
         <v>479</v>
       </c>
@@ -5300,14 +5446,17 @@
       <c r="I45" s="25"/>
       <c r="J45" s="24"/>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="22">
         <v>44</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B46),VLOOKUP(B46,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD1</v>
+      </c>
       <c r="D46" s="23" t="s">
         <v>480</v>
       </c>
@@ -5322,14 +5471,17 @@
       <c r="I46" s="25"/>
       <c r="J46" s="24"/>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="22">
         <v>45</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="23"/>
+      <c r="C47" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B47),VLOOKUP(B47,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD2</v>
+      </c>
       <c r="D47" s="23" t="s">
         <v>481</v>
       </c>
@@ -5344,14 +5496,17 @@
       <c r="I47" s="25"/>
       <c r="J47" s="24"/>
     </row>
-    <row r="48" spans="1:10" hidden="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="22">
         <v>46</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="23"/>
+      <c r="C48" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B48),VLOOKUP(B48,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD3</v>
+      </c>
       <c r="D48" s="23" t="s">
         <v>482</v>
       </c>
@@ -5366,14 +5521,17 @@
       <c r="I48" s="25"/>
       <c r="J48" s="24"/>
     </row>
-    <row r="49" spans="1:10" hidden="1">
+    <row r="49" spans="1:10">
       <c r="A49" s="22">
         <v>47</v>
       </c>
       <c r="B49" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="23"/>
+      <c r="C49" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B49),VLOOKUP(B49,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD4</v>
+      </c>
       <c r="D49" s="23" t="s">
         <v>483</v>
       </c>
@@ -5388,14 +5546,17 @@
       <c r="I49" s="25"/>
       <c r="J49" s="24"/>
     </row>
-    <row r="50" spans="1:10" hidden="1">
+    <row r="50" spans="1:10">
       <c r="A50" s="22">
         <v>48</v>
       </c>
       <c r="B50" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="23"/>
+      <c r="C50" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B50),VLOOKUP(B50,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PD5</v>
+      </c>
       <c r="D50" s="23" t="s">
         <v>484</v>
       </c>
@@ -5410,14 +5571,17 @@
       <c r="I50" s="25"/>
       <c r="J50" s="24"/>
     </row>
-    <row r="51" spans="1:10" hidden="1">
+    <row r="51" spans="1:10">
       <c r="A51" s="22">
         <v>49</v>
       </c>
       <c r="B51" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="23"/>
+      <c r="C51" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B51),VLOOKUP(B51,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>VBUST</v>
+      </c>
       <c r="D51" s="23" t="s">
         <v>17</v>
       </c>
@@ -5438,14 +5602,17 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1">
+    <row r="52" spans="1:10">
       <c r="A52" s="22">
         <v>50</v>
       </c>
       <c r="B52" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="23"/>
+      <c r="C52" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B52),VLOOKUP(B52,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>DN</v>
+      </c>
       <c r="D52" s="23" t="s">
         <v>238</v>
       </c>
@@ -5460,14 +5627,17 @@
         <v>527</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1">
+    <row r="53" spans="1:10">
       <c r="A53" s="22">
         <v>51</v>
       </c>
       <c r="B53" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="23"/>
+      <c r="C53" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B53),VLOOKUP(B53,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>DP</v>
+      </c>
       <c r="D53" s="23" t="s">
         <v>238</v>
       </c>
@@ -5482,14 +5652,17 @@
         <v>527</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1">
+    <row r="54" spans="1:10">
       <c r="A54" s="22">
         <v>52</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="23"/>
+      <c r="C54" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B54),VLOOKUP(B54,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D54" s="23" t="s">
         <v>17</v>
       </c>
@@ -5508,14 +5681,17 @@
       </c>
       <c r="J54" s="24"/>
     </row>
-    <row r="55" spans="1:10" hidden="1">
+    <row r="55" spans="1:10">
       <c r="A55" s="22">
         <v>53</v>
       </c>
       <c r="B55" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="23"/>
+      <c r="C55" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B55),VLOOKUP(B55,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D55" s="23" t="s">
         <v>15</v>
       </c>
@@ -5534,14 +5710,17 @@
       </c>
       <c r="J55" s="24"/>
     </row>
-    <row r="56" spans="1:10" hidden="1">
+    <row r="56" spans="1:10">
       <c r="A56" s="22">
         <v>54</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="23"/>
+      <c r="C56" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B56),VLOOKUP(B56,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D56" s="23" t="s">
         <v>283</v>
       </c>
@@ -5564,14 +5743,17 @@
         <v>280</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1">
+    <row r="57" spans="1:10">
       <c r="A57" s="22">
         <v>55</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="23"/>
+      <c r="C57" s="18">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B57),VLOOKUP(B57,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>0</v>
+      </c>
       <c r="D57" s="23" t="s">
         <v>283</v>
       </c>
@@ -5594,14 +5776,17 @@
         <v>280</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1">
+    <row r="58" spans="1:10">
       <c r="A58" s="22">
         <v>56</v>
       </c>
       <c r="B58" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="23"/>
+      <c r="C58" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B58),VLOOKUP(B58,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D58" s="23" t="s">
         <v>17</v>
       </c>
@@ -5620,14 +5805,17 @@
       </c>
       <c r="J58" s="24"/>
     </row>
-    <row r="59" spans="1:10" hidden="1">
+    <row r="59" spans="1:10">
       <c r="A59" s="22">
         <v>57</v>
       </c>
       <c r="B59" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="23"/>
+      <c r="C59" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B59),VLOOKUP(B59,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG2</v>
+      </c>
       <c r="D59" s="23" t="s">
         <v>173</v>
       </c>
@@ -5644,14 +5832,17 @@
         <v>259</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1">
+    <row r="60" spans="1:10">
       <c r="A60" s="22">
         <v>58</v>
       </c>
       <c r="B60" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="23"/>
+      <c r="C60" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B60),VLOOKUP(B60,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG3</v>
+      </c>
       <c r="D60" s="23" t="s">
         <v>174</v>
       </c>
@@ -5668,14 +5859,17 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1">
+    <row r="61" spans="1:10">
       <c r="A61" s="22">
         <v>59</v>
       </c>
       <c r="B61" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="23"/>
+      <c r="C61" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B61),VLOOKUP(B61,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG4</v>
+      </c>
       <c r="D61" s="23" t="s">
         <v>175</v>
       </c>
@@ -5692,14 +5886,17 @@
         <v>261</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1">
+    <row r="62" spans="1:10">
       <c r="A62" s="22">
         <v>60</v>
       </c>
       <c r="B62" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="23"/>
+      <c r="C62" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B62),VLOOKUP(B62,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG5</v>
+      </c>
       <c r="D62" s="23" t="s">
         <v>176</v>
       </c>
@@ -5716,14 +5913,17 @@
         <v>262</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1">
+    <row r="63" spans="1:10">
       <c r="A63" s="22">
         <v>61</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="23"/>
+      <c r="C63" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B63),VLOOKUP(B63,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG6</v>
+      </c>
       <c r="D63" s="23" t="s">
         <v>177</v>
       </c>
@@ -5740,14 +5940,17 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1">
+    <row r="64" spans="1:10">
       <c r="A64" s="22">
         <v>62</v>
       </c>
       <c r="B64" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C64" s="23"/>
+      <c r="C64" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B64),VLOOKUP(B64,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PG7</v>
+      </c>
       <c r="D64" s="23" t="s">
         <v>178</v>
       </c>
@@ -5764,14 +5967,17 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1">
+    <row r="65" spans="1:10">
       <c r="A65" s="22">
         <v>63</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C65" s="23"/>
+      <c r="C65" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B65),VLOOKUP(B65,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH0</v>
+      </c>
       <c r="D65" s="23" t="s">
         <v>179</v>
       </c>
@@ -5788,14 +5994,17 @@
         <v>265</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1">
+    <row r="66" spans="1:10">
       <c r="A66" s="22">
         <v>64</v>
       </c>
       <c r="B66" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C66" s="23"/>
+      <c r="C66" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B66),VLOOKUP(B66,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH1</v>
+      </c>
       <c r="D66" s="23" t="s">
         <v>180</v>
       </c>
@@ -5812,14 +6021,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1">
+    <row r="67" spans="1:10">
       <c r="A67" s="22">
         <v>65</v>
       </c>
       <c r="B67" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C67" s="23"/>
+      <c r="C67" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B67),VLOOKUP(B67,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH2</v>
+      </c>
       <c r="D67" s="23" t="s">
         <v>181</v>
       </c>
@@ -5836,14 +6048,17 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1">
+    <row r="68" spans="1:10">
       <c r="A68" s="22">
         <v>66</v>
       </c>
       <c r="B68" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C68" s="23"/>
+      <c r="C68" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B68),VLOOKUP(B68,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH3</v>
+      </c>
       <c r="D68" s="23" t="s">
         <v>182</v>
       </c>
@@ -5860,14 +6075,17 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1">
+    <row r="69" spans="1:10">
       <c r="A69" s="22">
         <v>67</v>
       </c>
       <c r="B69" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="23"/>
+      <c r="C69" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B69),VLOOKUP(B69,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH4</v>
+      </c>
       <c r="D69" s="23" t="s">
         <v>183</v>
       </c>
@@ -5884,14 +6102,17 @@
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1">
+    <row r="70" spans="1:10">
       <c r="A70" s="22">
         <v>68</v>
       </c>
       <c r="B70" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C70" s="23"/>
+      <c r="C70" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B70),VLOOKUP(B70,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH5</v>
+      </c>
       <c r="D70" s="23" t="s">
         <v>184</v>
       </c>
@@ -5908,14 +6129,17 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1">
+    <row r="71" spans="1:10">
       <c r="A71" s="22">
         <v>69</v>
       </c>
       <c r="B71" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="23"/>
+      <c r="C71" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B71),VLOOKUP(B71,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH6, XTAL1</v>
+      </c>
       <c r="D71" s="23" t="s">
         <v>185</v>
       </c>
@@ -5932,14 +6156,17 @@
         <v>271</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1">
+    <row r="72" spans="1:10">
       <c r="A72" s="22">
         <v>70</v>
       </c>
       <c r="B72" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="23"/>
+      <c r="C72" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B72),VLOOKUP(B72,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PH7, XTAL2</v>
+      </c>
       <c r="D72" s="23" t="s">
         <v>186</v>
       </c>
@@ -5956,14 +6183,17 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1">
+    <row r="73" spans="1:10">
       <c r="A73" s="22">
         <v>71</v>
       </c>
       <c r="B73" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C73" s="23"/>
+      <c r="C73" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B73),VLOOKUP(B73,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ0</v>
+      </c>
       <c r="D73" s="23" t="s">
         <v>187</v>
       </c>
@@ -5980,14 +6210,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1">
+    <row r="74" spans="1:10">
       <c r="A74" s="22">
         <v>72</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C74" s="23"/>
+      <c r="C74" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B74),VLOOKUP(B74,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ1, UVCON</v>
+      </c>
       <c r="D74" s="23" t="s">
         <v>188</v>
       </c>
@@ -6004,14 +6237,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1">
+    <row r="75" spans="1:10">
       <c r="A75" s="26">
         <v>73</v>
       </c>
       <c r="B75" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C75" s="27"/>
+      <c r="C75" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B75),VLOOKUP(B75,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ2</v>
+      </c>
       <c r="D75" s="27" t="s">
         <v>189</v>
       </c>
@@ -6028,14 +6264,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1">
+    <row r="76" spans="1:10">
       <c r="A76" s="26">
         <v>74</v>
       </c>
       <c r="B76" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="27"/>
+      <c r="C76" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B76),VLOOKUP(B76,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ3</v>
+      </c>
       <c r="D76" s="27" t="s">
         <v>190</v>
       </c>
@@ -6052,14 +6291,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1">
+    <row r="77" spans="1:10">
       <c r="A77" s="26">
         <v>75</v>
       </c>
       <c r="B77" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C77" s="27"/>
+      <c r="C77" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B77),VLOOKUP(B77,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D77" s="27" t="s">
         <v>15</v>
       </c>
@@ -6080,14 +6322,17 @@
       </c>
       <c r="J77" s="29"/>
     </row>
-    <row r="78" spans="1:10" hidden="1">
+    <row r="78" spans="1:10">
       <c r="A78" s="26">
         <v>76</v>
       </c>
       <c r="B78" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C78" s="27"/>
+      <c r="C78" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B78),VLOOKUP(B78,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D78" s="27" t="s">
         <v>17</v>
       </c>
@@ -6108,14 +6353,17 @@
       </c>
       <c r="J78" s="29"/>
     </row>
-    <row r="79" spans="1:10" hidden="1">
+    <row r="79" spans="1:10">
       <c r="A79" s="26">
         <v>77</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C79" s="27"/>
+      <c r="C79" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B79),VLOOKUP(B79,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ4</v>
+      </c>
       <c r="D79" s="27" t="s">
         <v>191</v>
       </c>
@@ -6132,14 +6380,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1">
+    <row r="80" spans="1:10">
       <c r="A80" s="26">
         <v>78</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="27"/>
+      <c r="C80" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B80),VLOOKUP(B80,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ5</v>
+      </c>
       <c r="D80" s="27" t="s">
         <v>192</v>
       </c>
@@ -6156,14 +6407,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1">
+    <row r="81" spans="1:10">
       <c r="A81" s="26">
         <v>79</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C81" s="27"/>
+      <c r="C81" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B81),VLOOKUP(B81,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ6</v>
+      </c>
       <c r="D81" s="27" t="s">
         <v>193</v>
       </c>
@@ -6180,14 +6434,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1">
+    <row r="82" spans="1:10">
       <c r="A82" s="26">
         <v>80</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="27"/>
+      <c r="C82" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B82),VLOOKUP(B82,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PJ7</v>
+      </c>
       <c r="D82" s="27" t="s">
         <v>194</v>
       </c>
@@ -6204,14 +6461,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1">
+    <row r="83" spans="1:10">
       <c r="A83" s="26">
         <v>81</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="27"/>
+      <c r="C83" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B83),VLOOKUP(B83,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK0</v>
+      </c>
       <c r="D83" s="27" t="s">
         <v>195</v>
       </c>
@@ -6228,14 +6488,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1">
+    <row r="84" spans="1:10">
       <c r="A84" s="26">
         <v>82</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="27"/>
+      <c r="C84" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B84),VLOOKUP(B84,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK1</v>
+      </c>
       <c r="D84" s="27" t="s">
         <v>196</v>
       </c>
@@ -6252,14 +6515,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1">
+    <row r="85" spans="1:10">
       <c r="A85" s="26">
         <v>83</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="27"/>
+      <c r="C85" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B85),VLOOKUP(B85,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK2</v>
+      </c>
       <c r="D85" s="27" t="s">
         <v>197</v>
       </c>
@@ -6276,14 +6542,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1">
+    <row r="86" spans="1:10">
       <c r="A86" s="26">
         <v>84</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="27"/>
+      <c r="C86" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B86),VLOOKUP(B86,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK3</v>
+      </c>
       <c r="D86" s="27" t="s">
         <v>198</v>
       </c>
@@ -6300,14 +6569,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1">
+    <row r="87" spans="1:10">
       <c r="A87" s="26">
         <v>85</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C87" s="27"/>
+      <c r="C87" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B87),VLOOKUP(B87,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK4</v>
+      </c>
       <c r="D87" s="27" t="s">
         <v>199</v>
       </c>
@@ -6324,14 +6596,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1">
+    <row r="88" spans="1:10">
       <c r="A88" s="26">
         <v>86</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C88" s="27"/>
+      <c r="C88" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B88),VLOOKUP(B88,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK5</v>
+      </c>
       <c r="D88" s="27" t="s">
         <v>200</v>
       </c>
@@ -6348,14 +6623,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1">
+    <row r="89" spans="1:10">
       <c r="A89" s="26">
         <v>87</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="27"/>
+      <c r="C89" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B89),VLOOKUP(B89,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK6</v>
+      </c>
       <c r="D89" s="27" t="s">
         <v>201</v>
       </c>
@@ -6372,14 +6650,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1">
+    <row r="90" spans="1:10">
       <c r="A90" s="26">
         <v>88</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C90" s="27"/>
+      <c r="C90" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B90),VLOOKUP(B90,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PK7</v>
+      </c>
       <c r="D90" s="27" t="s">
         <v>202</v>
       </c>
@@ -6396,14 +6677,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1">
+    <row r="91" spans="1:10">
       <c r="A91" s="26">
         <v>89</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C91" s="27"/>
+      <c r="C91" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B91),VLOOKUP(B91,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL0</v>
+      </c>
       <c r="D91" s="27" t="s">
         <v>203</v>
       </c>
@@ -6420,14 +6704,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1">
+    <row r="92" spans="1:10">
       <c r="A92" s="26">
         <v>90</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C92" s="27"/>
+      <c r="C92" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B92),VLOOKUP(B92,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL1</v>
+      </c>
       <c r="D92" s="27" t="s">
         <v>204</v>
       </c>
@@ -6444,14 +6731,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1">
+    <row r="93" spans="1:10">
       <c r="A93" s="26">
         <v>91</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C93" s="27"/>
+      <c r="C93" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B93),VLOOKUP(B93,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL2</v>
+      </c>
       <c r="D93" s="27" t="s">
         <v>205</v>
       </c>
@@ -6468,14 +6758,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1">
+    <row r="94" spans="1:10">
       <c r="A94" s="26">
         <v>92</v>
       </c>
       <c r="B94" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C94" s="27"/>
+      <c r="C94" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B94),VLOOKUP(B94,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL3</v>
+      </c>
       <c r="D94" s="27" t="s">
         <v>206</v>
       </c>
@@ -6492,14 +6785,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1">
+    <row r="95" spans="1:10">
       <c r="A95" s="26">
         <v>93</v>
       </c>
       <c r="B95" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C95" s="27"/>
+      <c r="C95" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B95),VLOOKUP(B95,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL4</v>
+      </c>
       <c r="D95" s="27" t="s">
         <v>207</v>
       </c>
@@ -6516,14 +6812,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1">
+    <row r="96" spans="1:10">
       <c r="A96" s="26">
         <v>94</v>
       </c>
       <c r="B96" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C96" s="27"/>
+      <c r="C96" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B96),VLOOKUP(B96,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL5</v>
+      </c>
       <c r="D96" s="27" t="s">
         <v>208</v>
       </c>
@@ -6540,14 +6839,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1">
+    <row r="97" spans="1:10">
       <c r="A97" s="26">
         <v>95</v>
       </c>
       <c r="B97" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C97" s="27"/>
+      <c r="C97" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B97),VLOOKUP(B97,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL6</v>
+      </c>
       <c r="D97" s="27" t="s">
         <v>209</v>
       </c>
@@ -6564,14 +6866,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1">
+    <row r="98" spans="1:10">
       <c r="A98" s="26">
         <v>96</v>
       </c>
       <c r="B98" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C98" s="27"/>
+      <c r="C98" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B98),VLOOKUP(B98,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PL7</v>
+      </c>
       <c r="D98" s="27" t="s">
         <v>210</v>
       </c>
@@ -6588,14 +6893,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1">
+    <row r="99" spans="1:10">
       <c r="A99" s="26">
         <v>97</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C99" s="27"/>
+      <c r="C99" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B99),VLOOKUP(B99,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM0</v>
+      </c>
       <c r="D99" s="27" t="s">
         <v>211</v>
       </c>
@@ -6612,14 +6920,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1">
+    <row r="100" spans="1:10">
       <c r="A100" s="26">
         <v>98</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C100" s="27"/>
+      <c r="C100" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B100),VLOOKUP(B100,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM1</v>
+      </c>
       <c r="D100" s="27" t="s">
         <v>212</v>
       </c>
@@ -6636,14 +6947,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1">
+    <row r="101" spans="1:10">
       <c r="A101" s="26">
         <v>99</v>
       </c>
       <c r="B101" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="C101" s="27"/>
+      <c r="C101" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B101),VLOOKUP(B101,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM2</v>
+      </c>
       <c r="D101" s="27" t="s">
         <v>213</v>
       </c>
@@ -6660,14 +6974,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1">
+    <row r="102" spans="1:10">
       <c r="A102" s="26">
         <v>100</v>
       </c>
       <c r="B102" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C102" s="27"/>
+      <c r="C102" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B102),VLOOKUP(B102,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM3</v>
+      </c>
       <c r="D102" s="27" t="s">
         <v>214</v>
       </c>
@@ -6684,14 +7001,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1">
+    <row r="103" spans="1:10">
       <c r="A103" s="26">
         <v>101</v>
       </c>
       <c r="B103" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C103" s="27"/>
+      <c r="C103" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B103),VLOOKUP(B103,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM4</v>
+      </c>
       <c r="D103" s="27" t="s">
         <v>215</v>
       </c>
@@ -6708,14 +7028,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1">
+    <row r="104" spans="1:10">
       <c r="A104" s="26">
         <v>102</v>
       </c>
       <c r="B104" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C104" s="27"/>
+      <c r="C104" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B104),VLOOKUP(B104,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM5</v>
+      </c>
       <c r="D104" s="27" t="s">
         <v>216</v>
       </c>
@@ -6732,14 +7055,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1">
+    <row r="105" spans="1:10">
       <c r="A105" s="26">
         <v>103</v>
       </c>
       <c r="B105" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C105" s="27"/>
+      <c r="C105" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B105),VLOOKUP(B105,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D105" s="27" t="s">
         <v>15</v>
       </c>
@@ -6760,14 +7086,17 @@
       </c>
       <c r="J105" s="29"/>
     </row>
-    <row r="106" spans="1:10" hidden="1">
+    <row r="106" spans="1:10">
       <c r="A106" s="26">
         <v>104</v>
       </c>
       <c r="B106" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="C106" s="27"/>
+      <c r="C106" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B106),VLOOKUP(B106,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D106" s="27" t="s">
         <v>17</v>
       </c>
@@ -6788,14 +7117,17 @@
       </c>
       <c r="J106" s="29"/>
     </row>
-    <row r="107" spans="1:10" hidden="1">
+    <row r="107" spans="1:10">
       <c r="A107" s="26">
         <v>105</v>
       </c>
       <c r="B107" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C107" s="27"/>
+      <c r="C107" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B107),VLOOKUP(B107,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM6</v>
+      </c>
       <c r="D107" s="27" t="s">
         <v>217</v>
       </c>
@@ -6812,14 +7144,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1">
+    <row r="108" spans="1:10">
       <c r="A108" s="26">
         <v>106</v>
       </c>
       <c r="B108" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C108" s="27"/>
+      <c r="C108" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B108),VLOOKUP(B108,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PM7</v>
+      </c>
       <c r="D108" s="27" t="s">
         <v>218</v>
       </c>
@@ -6843,7 +7178,10 @@
       <c r="B109" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C109" s="27"/>
+      <c r="C109" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B109),VLOOKUP(B109,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN0</v>
+      </c>
       <c r="D109" s="27" t="s">
         <v>221</v>
       </c>
@@ -6871,7 +7209,10 @@
       <c r="B110" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="C110" s="27"/>
+      <c r="C110" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B110),VLOOKUP(B110,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN1</v>
+      </c>
       <c r="D110" s="27" t="s">
         <v>222</v>
       </c>
@@ -6899,7 +7240,10 @@
       <c r="B111" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C111" s="31"/>
+      <c r="C111" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B111),VLOOKUP(B111,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN2</v>
+      </c>
       <c r="D111" s="31" t="s">
         <v>284</v>
       </c>
@@ -6923,8 +7267,9 @@
       <c r="B112" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="31" t="s">
-        <v>424</v>
+      <c r="C112" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B112),VLOOKUP(B112,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN3</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>226</v>
@@ -6955,8 +7300,9 @@
       <c r="B113" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C113" s="31" t="s">
-        <v>425</v>
+      <c r="C113" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B113),VLOOKUP(B113,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN4</v>
       </c>
       <c r="D113" s="31" t="s">
         <v>228</v>
@@ -6987,8 +7333,9 @@
       <c r="B114" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="C114" s="31" t="s">
-        <v>426</v>
+      <c r="C114" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B114),VLOOKUP(B114,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN5</v>
       </c>
       <c r="D114" s="31" t="s">
         <v>230</v>
@@ -7019,8 +7366,9 @@
       <c r="B115" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C115" s="31" t="s">
-        <v>427</v>
+      <c r="C115" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B115),VLOOKUP(B115,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN6</v>
       </c>
       <c r="D115" s="31" t="s">
         <v>232</v>
@@ -7044,14 +7392,17 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1">
+    <row r="116" spans="1:10">
       <c r="A116" s="30">
         <v>114</v>
       </c>
       <c r="B116" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C116" s="31"/>
+      <c r="C116" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B116),VLOOKUP(B116,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PN7</v>
+      </c>
       <c r="D116" s="31" t="s">
         <v>238</v>
       </c>
@@ -7064,14 +7415,17 @@
       <c r="I116" s="32"/>
       <c r="J116" s="33"/>
     </row>
-    <row r="117" spans="1:10" hidden="1">
+    <row r="117" spans="1:10">
       <c r="A117" s="30">
         <v>115</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C117" s="31"/>
+      <c r="C117" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B117),VLOOKUP(B117,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP0</v>
+      </c>
       <c r="D117" s="31" t="s">
         <v>238</v>
       </c>
@@ -7084,14 +7438,17 @@
       <c r="I117" s="32"/>
       <c r="J117" s="33"/>
     </row>
-    <row r="118" spans="1:10" hidden="1">
+    <row r="118" spans="1:10">
       <c r="A118" s="30">
         <v>116</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C118" s="31"/>
+      <c r="C118" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B118),VLOOKUP(B118,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP1</v>
+      </c>
       <c r="D118" s="31" t="s">
         <v>238</v>
       </c>
@@ -7104,14 +7461,17 @@
       <c r="I118" s="32"/>
       <c r="J118" s="33"/>
     </row>
-    <row r="119" spans="1:10" hidden="1">
+    <row r="119" spans="1:10">
       <c r="A119" s="30">
         <v>117</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C119" s="31"/>
+      <c r="C119" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B119),VLOOKUP(B119,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP2</v>
+      </c>
       <c r="D119" s="31" t="s">
         <v>238</v>
       </c>
@@ -7124,14 +7484,17 @@
       <c r="I119" s="32"/>
       <c r="J119" s="33"/>
     </row>
-    <row r="120" spans="1:10" hidden="1">
+    <row r="120" spans="1:10">
       <c r="A120" s="30">
         <v>118</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C120" s="31"/>
+      <c r="C120" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B120),VLOOKUP(B120,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D120" s="31" t="s">
         <v>15</v>
       </c>
@@ -7152,14 +7515,17 @@
       </c>
       <c r="J120" s="33"/>
     </row>
-    <row r="121" spans="1:10" hidden="1">
+    <row r="121" spans="1:10">
       <c r="A121" s="30">
         <v>119</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C121" s="31"/>
+      <c r="C121" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B121),VLOOKUP(B121,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D121" s="31" t="s">
         <v>17</v>
       </c>
@@ -7180,14 +7546,17 @@
       </c>
       <c r="J121" s="33"/>
     </row>
-    <row r="122" spans="1:10" hidden="1">
+    <row r="122" spans="1:10">
       <c r="A122" s="30">
         <v>120</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C122" s="31"/>
+      <c r="C122" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B122),VLOOKUP(B122,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP3</v>
+      </c>
       <c r="D122" s="31" t="s">
         <v>485</v>
       </c>
@@ -7202,14 +7571,17 @@
       <c r="I122" s="32"/>
       <c r="J122" s="33"/>
     </row>
-    <row r="123" spans="1:10" hidden="1">
+    <row r="123" spans="1:10">
       <c r="A123" s="30">
         <v>121</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="C123" s="31"/>
+      <c r="C123" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B123),VLOOKUP(B123,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP4</v>
+      </c>
       <c r="D123" s="31" t="s">
         <v>486</v>
       </c>
@@ -7224,14 +7596,17 @@
       <c r="I123" s="32"/>
       <c r="J123" s="33"/>
     </row>
-    <row r="124" spans="1:10" hidden="1">
+    <row r="124" spans="1:10">
       <c r="A124" s="30">
         <v>122</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C124" s="31"/>
+      <c r="C124" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B124),VLOOKUP(B124,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP5</v>
+      </c>
       <c r="D124" s="31" t="s">
         <v>487</v>
       </c>
@@ -7246,14 +7621,17 @@
       <c r="I124" s="32"/>
       <c r="J124" s="33"/>
     </row>
-    <row r="125" spans="1:10" hidden="1">
+    <row r="125" spans="1:10">
       <c r="A125" s="30">
         <v>123</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C125" s="31"/>
+      <c r="C125" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B125),VLOOKUP(B125,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP6</v>
+      </c>
       <c r="D125" s="31" t="s">
         <v>488</v>
       </c>
@@ -7268,14 +7646,17 @@
       <c r="I125" s="32"/>
       <c r="J125" s="33"/>
     </row>
-    <row r="126" spans="1:10" hidden="1">
+    <row r="126" spans="1:10">
       <c r="A126" s="30">
         <v>124</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="C126" s="31"/>
+      <c r="C126" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B126),VLOOKUP(B126,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PP7</v>
+      </c>
       <c r="D126" s="31" t="s">
         <v>489</v>
       </c>
@@ -7290,14 +7671,17 @@
       <c r="I126" s="32"/>
       <c r="J126" s="33"/>
     </row>
-    <row r="127" spans="1:10" hidden="1">
+    <row r="127" spans="1:10">
       <c r="A127" s="30">
         <v>125</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C127" s="31"/>
+      <c r="C127" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B127),VLOOKUP(B127,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ0</v>
+      </c>
       <c r="D127" s="31" t="s">
         <v>490</v>
       </c>
@@ -7312,14 +7696,17 @@
       <c r="I127" s="32"/>
       <c r="J127" s="33"/>
     </row>
-    <row r="128" spans="1:10" hidden="1">
+    <row r="128" spans="1:10">
       <c r="A128" s="30">
         <v>126</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C128" s="31"/>
+      <c r="C128" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B128),VLOOKUP(B128,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ1</v>
+      </c>
       <c r="D128" s="31" t="s">
         <v>491</v>
       </c>
@@ -7334,14 +7721,17 @@
       <c r="I128" s="32"/>
       <c r="J128" s="33"/>
     </row>
-    <row r="129" spans="1:10" hidden="1">
+    <row r="129" spans="1:10">
       <c r="A129" s="30">
         <v>127</v>
       </c>
       <c r="B129" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C129" s="31"/>
+      <c r="C129" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B129),VLOOKUP(B129,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ2</v>
+      </c>
       <c r="D129" s="31" t="s">
         <v>492</v>
       </c>
@@ -7356,14 +7746,17 @@
       <c r="I129" s="32"/>
       <c r="J129" s="33"/>
     </row>
-    <row r="130" spans="1:10" hidden="1">
+    <row r="130" spans="1:10">
       <c r="A130" s="30">
         <v>128</v>
       </c>
       <c r="B130" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="C130" s="31"/>
+      <c r="C130" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B130),VLOOKUP(B130,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ3</v>
+      </c>
       <c r="D130" s="31" t="s">
         <v>493</v>
       </c>
@@ -7378,14 +7771,17 @@
       <c r="I130" s="32"/>
       <c r="J130" s="33"/>
     </row>
-    <row r="131" spans="1:10" hidden="1">
+    <row r="131" spans="1:10">
       <c r="A131" s="30">
         <v>129</v>
       </c>
       <c r="B131" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C131" s="31"/>
+      <c r="C131" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B131),VLOOKUP(B131,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ4</v>
+      </c>
       <c r="D131" s="31" t="s">
         <v>494</v>
       </c>
@@ -7400,14 +7796,17 @@
       <c r="I131" s="32"/>
       <c r="J131" s="33"/>
     </row>
-    <row r="132" spans="1:10" hidden="1">
+    <row r="132" spans="1:10">
       <c r="A132" s="30">
         <v>130</v>
       </c>
       <c r="B132" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="C132" s="31"/>
+      <c r="C132" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B132),VLOOKUP(B132,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ5</v>
+      </c>
       <c r="D132" s="31" t="s">
         <v>529</v>
       </c>
@@ -7424,14 +7823,17 @@
         <v>534</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1">
+    <row r="133" spans="1:10">
       <c r="A133" s="30">
         <v>131</v>
       </c>
       <c r="B133" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C133" s="31"/>
+      <c r="C133" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B133),VLOOKUP(B133,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ6</v>
+      </c>
       <c r="D133" s="31" t="s">
         <v>530</v>
       </c>
@@ -7448,14 +7850,17 @@
         <v>534</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1">
+    <row r="134" spans="1:10">
       <c r="A134" s="30">
         <v>132</v>
       </c>
       <c r="B134" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="C134" s="31"/>
+      <c r="C134" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B134),VLOOKUP(B134,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PQ7</v>
+      </c>
       <c r="D134" s="31" t="s">
         <v>531</v>
       </c>
@@ -7472,14 +7877,17 @@
         <v>534</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1">
+    <row r="135" spans="1:10">
       <c r="A135" s="30">
         <v>133</v>
       </c>
       <c r="B135" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="C135" s="31"/>
+      <c r="C135" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B135),VLOOKUP(B135,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA0</v>
+      </c>
       <c r="D135" s="31" t="s">
         <v>532</v>
       </c>
@@ -7496,14 +7904,17 @@
         <v>534</v>
       </c>
     </row>
-    <row r="136" spans="1:10" hidden="1">
+    <row r="136" spans="1:10">
       <c r="A136" s="30">
         <v>134</v>
       </c>
       <c r="B136" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="C136" s="31"/>
+      <c r="C136" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B136),VLOOKUP(B136,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA1</v>
+      </c>
       <c r="D136" s="31" t="s">
         <v>238</v>
       </c>
@@ -7516,14 +7927,17 @@
       <c r="I136" s="32"/>
       <c r="J136" s="33"/>
     </row>
-    <row r="137" spans="1:10" hidden="1">
+    <row r="137" spans="1:10">
       <c r="A137" s="30">
         <v>135</v>
       </c>
       <c r="B137" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C137" s="31"/>
+      <c r="C137" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B137),VLOOKUP(B137,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA2</v>
+      </c>
       <c r="D137" s="31" t="s">
         <v>238</v>
       </c>
@@ -7536,14 +7950,17 @@
       <c r="I137" s="32"/>
       <c r="J137" s="33"/>
     </row>
-    <row r="138" spans="1:10" hidden="1">
+    <row r="138" spans="1:10">
       <c r="A138" s="30">
         <v>136</v>
       </c>
       <c r="B138" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C138" s="31"/>
+      <c r="C138" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B138),VLOOKUP(B138,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA3</v>
+      </c>
       <c r="D138" s="31" t="s">
         <v>238</v>
       </c>
@@ -7556,14 +7973,17 @@
       <c r="I138" s="32"/>
       <c r="J138" s="33"/>
     </row>
-    <row r="139" spans="1:10" hidden="1">
+    <row r="139" spans="1:10">
       <c r="A139" s="30">
         <v>137</v>
       </c>
       <c r="B139" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C139" s="31"/>
+      <c r="C139" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B139),VLOOKUP(B139,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA4</v>
+      </c>
       <c r="D139" s="31" t="s">
         <v>238</v>
       </c>
@@ -7576,14 +7996,17 @@
       <c r="I139" s="32"/>
       <c r="J139" s="33"/>
     </row>
-    <row r="140" spans="1:10" hidden="1">
+    <row r="140" spans="1:10">
       <c r="A140" s="30">
         <v>138</v>
       </c>
       <c r="B140" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C140" s="31"/>
+      <c r="C140" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B140),VLOOKUP(B140,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA5</v>
+      </c>
       <c r="D140" s="31" t="s">
         <v>238</v>
       </c>
@@ -7596,14 +8019,17 @@
       <c r="I140" s="32"/>
       <c r="J140" s="33"/>
     </row>
-    <row r="141" spans="1:10" hidden="1">
+    <row r="141" spans="1:10">
       <c r="A141" s="30">
         <v>139</v>
       </c>
       <c r="B141" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="C141" s="31"/>
+      <c r="C141" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B141),VLOOKUP(B141,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PDATA6</v>
+      </c>
       <c r="D141" s="31" t="s">
         <v>238</v>
       </c>
@@ -7616,14 +8042,17 @@
       <c r="I141" s="32"/>
       <c r="J141" s="33"/>
     </row>
-    <row r="142" spans="1:10" hidden="1">
+    <row r="142" spans="1:10">
       <c r="A142" s="30">
         <v>140</v>
       </c>
       <c r="B142" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="C142" s="31"/>
+      <c r="C142" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B142),VLOOKUP(B142,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE0, TOSC1</v>
+      </c>
       <c r="D142" s="31" t="s">
         <v>163</v>
       </c>
@@ -7640,14 +8069,17 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:10" hidden="1">
+    <row r="143" spans="1:10">
       <c r="A143" s="30">
         <v>141</v>
       </c>
       <c r="B143" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C143" s="31"/>
+      <c r="C143" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B143),VLOOKUP(B143,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE1, TOSC2</v>
+      </c>
       <c r="D143" s="31" t="s">
         <v>162</v>
       </c>
@@ -7664,14 +8096,17 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:10" hidden="1">
+    <row r="144" spans="1:10">
       <c r="A144" s="30">
         <v>142</v>
       </c>
       <c r="B144" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="C144" s="31"/>
+      <c r="C144" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B144),VLOOKUP(B144,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>---</v>
+      </c>
       <c r="D144" s="31" t="s">
         <v>172</v>
       </c>
@@ -7688,14 +8123,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1">
+    <row r="145" spans="1:10">
       <c r="A145" s="30">
         <v>143</v>
       </c>
       <c r="B145" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C145" s="31"/>
+      <c r="C145" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B145),VLOOKUP(B145,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE2</v>
+      </c>
       <c r="D145" s="31" t="s">
         <v>164</v>
       </c>
@@ -7712,14 +8150,17 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1">
+    <row r="146" spans="1:10">
       <c r="A146" s="30">
         <v>144</v>
       </c>
       <c r="B146" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C146" s="31"/>
+      <c r="C146" s="18" t="str">
+        <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B146),VLOOKUP(B146,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
+        <v>PE3</v>
+      </c>
       <c r="D146" s="31" t="s">
         <v>165</v>
       </c>
@@ -7880,7 +8321,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="153" spans="1:10" ht="15.75" thickBot="1">
       <c r="A153" s="6"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -7902,6 +8343,7 @@
         <v>320</v>
       </c>
     </row>
+    <row r="154" spans="1:10" ht="15.75" thickTop="1"/>
     <row r="155" spans="1:10">
       <c r="A155" s="10" t="s">
         <v>322</v>
@@ -7910,11 +8352,7 @@
   </sheetData>
   <autoFilter ref="A2:J153">
     <filterColumn colId="2"/>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="SHIELD-DATA-TRANSFER"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="4"/>
     <filterColumn colId="6"/>
     <filterColumn colId="8"/>
   </autoFilter>
@@ -7933,8 +8371,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9023,7 +9461,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="Z16:BH92"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BH45" sqref="BH45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated pin assignment documentation related to testing undertaken.
</commit_message>
<xml_diff>
--- a/hardware/TouchShield-Pin-Assignment.xlsx
+++ b/hardware/TouchShield-Pin-Assignment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28620" windowHeight="14955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Assignment" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="536">
   <si>
     <t>PIN</t>
   </si>
@@ -1624,6 +1624,9 @@
   </si>
   <si>
     <t>Comes out to suitable header for Target Data on QT600 interface board</t>
+  </si>
+  <si>
+    <t>QT-DEBUG</t>
   </si>
 </sst>
 </file>
@@ -2188,6 +2191,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2195,9 +2201,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2407,13 +2410,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2423,8 +2426,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590801" y="6477000"/>
-          <a:ext cx="2590800" cy="1457325"/>
+          <a:off x="2667001" y="6667500"/>
+          <a:ext cx="2667000" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2464,13 +2467,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2480,8 +2483,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2266950" y="8743950"/>
-          <a:ext cx="3238500" cy="1457325"/>
+          <a:off x="2333625" y="9001125"/>
+          <a:ext cx="3333750" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -2630,13 +2633,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161133</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>796</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2682,13 +2685,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2734,13 +2737,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>82551</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2786,13 +2789,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2802,8 +2805,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6315075" y="8743950"/>
-          <a:ext cx="3238500" cy="1457325"/>
+          <a:off x="6500813" y="9001125"/>
+          <a:ext cx="3333750" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -2848,13 +2851,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2898,13 +2901,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161132</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>795</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2950,13 +2953,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>80964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3003,13 +3006,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>57</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3019,8 +3022,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6638925" y="11010900"/>
-          <a:ext cx="2590800" cy="1457325"/>
+          <a:off x="6834188" y="11334750"/>
+          <a:ext cx="2667000" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartPredefinedProcess">
           <a:avLst/>
@@ -3065,13 +3068,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3081,8 +3084,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590800" y="11010900"/>
-          <a:ext cx="2590800" cy="1457325"/>
+          <a:off x="2667000" y="11334750"/>
+          <a:ext cx="2667000" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartPredefinedProcess">
           <a:avLst/>
@@ -3127,13 +3130,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>161132</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>795</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3179,13 +3182,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3195,8 +3198,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6800850" y="17811750"/>
-          <a:ext cx="2266950" cy="647700"/>
+          <a:off x="7000875" y="18335625"/>
+          <a:ext cx="2333625" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
           <a:avLst/>
@@ -3236,13 +3239,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>161132</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>795</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3254,8 +3257,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="7529513" y="12873037"/>
-          <a:ext cx="809625" cy="1588"/>
+          <a:off x="7748589" y="13249274"/>
+          <a:ext cx="833437" cy="6351"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -3287,13 +3290,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3303,8 +3306,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6315075" y="13277850"/>
-          <a:ext cx="3238500" cy="1457325"/>
+          <a:off x="6500813" y="13668375"/>
+          <a:ext cx="3333750" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -3349,13 +3352,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>57</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3365,8 +3368,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6638925" y="15544800"/>
-          <a:ext cx="2590800" cy="1457325"/>
+          <a:off x="6834188" y="16002000"/>
+          <a:ext cx="2667000" cy="1500188"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartPredefinedProcess">
           <a:avLst/>
@@ -3413,13 +3416,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>161132</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>795</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3465,13 +3468,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>161132</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>795</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3952,6 +3955,119 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>163284</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Flowchart: Decision 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="6694714"/>
+          <a:ext cx="3265714" cy="1469570"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Host MCU requests data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>?</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Elbow Connector 54"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3429001" y="6204857"/>
+          <a:ext cx="979715" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4245,8 +4361,8 @@
   </sheetPr>
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4263,21 +4379,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickTop="1" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="45" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="46"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:10" s="43" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="40" t="s">
@@ -4343,7 +4459,7 @@
       <c r="B4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="48" t="str">
+      <c r="C4" s="45" t="str">
         <f>IF(COUNTIF('STK600-RCUC3C0-36 Routing Card'!$A$2:$A$134,B4),VLOOKUP(B4,'STK600-RCUC3C0-36 Routing Card'!$A$2:$B$134,2,FALSE),"---")</f>
         <v>PA1, TDI</v>
       </c>
@@ -7816,7 +7932,9 @@
       <c r="F132" s="31" t="s">
         <v>533</v>
       </c>
-      <c r="G132" s="31"/>
+      <c r="G132" s="31" t="s">
+        <v>535</v>
+      </c>
       <c r="H132" s="31"/>
       <c r="I132" s="32"/>
       <c r="J132" s="33" t="s">
@@ -7843,7 +7961,9 @@
       <c r="F133" s="31" t="s">
         <v>533</v>
       </c>
-      <c r="G133" s="31"/>
+      <c r="G133" s="31" t="s">
+        <v>535</v>
+      </c>
       <c r="H133" s="31"/>
       <c r="I133" s="32"/>
       <c r="J133" s="33" t="s">
@@ -7870,7 +7990,9 @@
       <c r="F134" s="31" t="s">
         <v>533</v>
       </c>
-      <c r="G134" s="31"/>
+      <c r="G134" s="31" t="s">
+        <v>535</v>
+      </c>
       <c r="H134" s="31"/>
       <c r="I134" s="32"/>
       <c r="J134" s="33" t="s">
@@ -7897,7 +8019,9 @@
       <c r="F135" s="31" t="s">
         <v>533</v>
       </c>
-      <c r="G135" s="31"/>
+      <c r="G135" s="31" t="s">
+        <v>535</v>
+      </c>
       <c r="H135" s="31"/>
       <c r="I135" s="32"/>
       <c r="J135" s="33" t="s">
@@ -8371,7 +8495,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
@@ -9459,10 +9583,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="Z16:BH92"/>
+  <dimension ref="Z16:BH127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BH45" sqref="BH45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AR52" sqref="AR52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -9483,31 +9607,31 @@
         <v>460</v>
       </c>
     </row>
-    <row r="54" spans="26:51" ht="12.75" customHeight="1">
-      <c r="AY54" s="44" t="s">
+    <row r="89" spans="35:51" ht="12.75" customHeight="1">
+      <c r="AY89" s="44" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="58" spans="26:51" ht="12.75" customHeight="1">
-      <c r="AI58" s="44" t="s">
+    <row r="93" spans="35:51" ht="12.75" customHeight="1">
+      <c r="AI93" s="44" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="64" spans="26:51" ht="12.75" customHeight="1">
-      <c r="Z64" s="44" t="s">
+    <row r="99" spans="26:51" ht="12.75" customHeight="1">
+      <c r="Z99" s="44" t="s">
         <v>460</v>
       </c>
-      <c r="AY64" s="44" t="s">
+      <c r="AY99" s="44" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="86" spans="51:60" ht="12.75" customHeight="1">
-      <c r="BH86" s="44" t="s">
+    <row r="121" spans="51:60" ht="12.75" customHeight="1">
+      <c r="BH121" s="44" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="92" spans="51:60" ht="12.75" customHeight="1">
-      <c r="AY92" s="44" t="s">
+    <row r="127" spans="51:60" ht="12.75" customHeight="1">
+      <c r="AY127" s="44" t="s">
         <v>460</v>
       </c>
     </row>

</xml_diff>